<commit_message>
Add Logout Functionality Test
</commit_message>
<xml_diff>
--- a/Test Cases of pickaboo.com(Full & Final ).xlsx
+++ b/Test Cases of pickaboo.com(Full & Final ).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SQA2\Projects\Test Cases of pickaboo.com(Full &amp; Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD34A61-29D2-420F-B503-64141CA7F0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3816D64B-EC22-4DF0-86E1-27F7C675592C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="744" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="744" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="8" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="290">
   <si>
     <t>Project Name</t>
   </si>
@@ -1461,18 +1461,6 @@
     <t>TC_LF_022</t>
   </si>
   <si>
-    <t>TC_LF_023</t>
-  </si>
-  <si>
-    <t>TC_LF_024</t>
-  </si>
-  <si>
-    <t>TC_LF_025</t>
-  </si>
-  <si>
-    <t>TC_LF_026</t>
-  </si>
-  <si>
     <t>Verify the number of unsuccessful login attemps</t>
   </si>
   <si>
@@ -1884,13 +1872,165 @@
       <t xml:space="preserve"> into the Password field
 4. Click to 'Login' button</t>
     </r>
+  </si>
+  <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
+    <t>TC_LG_001</t>
+  </si>
+  <si>
+    <t>https://www.pickaboo.com/logout/</t>
+  </si>
+  <si>
+    <t>TS_003
+Logout Functionality</t>
+  </si>
+  <si>
+    <t>1. Open the Application
+2. User is logged In</t>
+  </si>
+  <si>
+    <t>Pre-requisites/Pre-Condition</t>
+  </si>
+  <si>
+    <t>Verify logging out by selection Logout option from 'My Account' drop Manu</t>
+  </si>
+  <si>
+    <t>Verify the application session status, after logging and closing the browser without login out</t>
+  </si>
+  <si>
+    <t>Verify logout from an Account from single place after logging into it from different places</t>
+  </si>
+  <si>
+    <t>Verify the Logout functionality in all the supported enviroments</t>
+  </si>
+  <si>
+    <t>Verify the logout using URL</t>
+  </si>
+  <si>
+    <t>Verify that if a user clicks on the back button of the browser after logout, the user should not be able to be redirected to a logged in mode application.</t>
+  </si>
+  <si>
+    <t>Verify that if the user clicks on the log out button then the user should be redirected on the home screen page.</t>
+  </si>
+  <si>
+    <t>Verify  After logout, try to re-login with the same or different account it’s allowing or not.</t>
+  </si>
+  <si>
+    <t>TC_LG_002</t>
+  </si>
+  <si>
+    <t>TC_LG_003</t>
+  </si>
+  <si>
+    <t>TC_LG_004</t>
+  </si>
+  <si>
+    <t>TC_LG_005</t>
+  </si>
+  <si>
+    <t>TC_LG_006</t>
+  </si>
+  <si>
+    <t>TC_LG_007</t>
+  </si>
+  <si>
+    <t>TC_LG_008</t>
+  </si>
+  <si>
+    <t>1. Click 'My Acount' Dropmenu 
+2. Select 'Logout' option and Click</t>
+  </si>
+  <si>
+    <t>1. User should be taken to the account logout page.
+2. User should be taken to the Home Page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click 'My Acount' Dropmenu 
+2. Select 'Logout' option and Click
+3. Click 'Login' menu
+4. Insert valid 'Mobile Number/Email' and 'Password' 
+5. Click on 'Login' button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Close the Browser without Logging out.
+2. Open the Browser again and navigate the application </t>
+  </si>
+  <si>
+    <t>1. Application should not get looged out, instead the user loggedin session need to be maintained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click 'My Acount' Dropmenu 
+2. Select 'Logout' option and Click
+</t>
+  </si>
+  <si>
+    <t>1. The user should not be able to be redirected to a logged in mode application.</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL 
+2. User is logged in Firefox Browser of your laptop.
+3. User is logged in with the same of step 2 in Chrome Browser of your Mobile device.</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Dropmenu in Firefox Browser option
+2. Select on 'Logout' option
+3. Perform any operation which requires the user to log, say navigaiton to Address Book page in the Chrome Browser of Mobile Device</t>
+  </si>
+  <si>
+    <t>1. User should be logged Out in Mobile device too, instead of getting navigated to the Address book page.</t>
+  </si>
+  <si>
+    <t>1. Copy the url (https://www.pickaboo.com/logout/
+2. Pase on URL bar and enter.</t>
+  </si>
+  <si>
+    <t>1. User should logged out</t>
+  </si>
+  <si>
+    <t>1. Logout functionality should work correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t>1. User is taken to the account  logout page.
+2. User is be redirect to Home Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User should be taken to the account logout page.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is taken to the account  logout page.
+</t>
+  </si>
+  <si>
+    <t>1. User is allow to login and  redirect on Home Page.</t>
+  </si>
+  <si>
+    <t>1. User should be allow to login again redirect on Home Page.</t>
+  </si>
+  <si>
+    <t>1. Application is not get looged out, 
+2. Session is runnigh</t>
+  </si>
+  <si>
+    <t>1. The user is not be able to be redirected to a logged in mode application.</t>
+  </si>
+  <si>
+    <t>1. User is not geeting Logout from others devices at a time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is not able to logout </t>
+  </si>
+  <si>
+    <t>Failed due to defect#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1941,6 +2081,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1993,7 +2140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2040,6 +2187,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2047,7 +2216,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2122,9 +2291,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2132,6 +2298,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2145,24 +2323,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2462,10 +2657,10 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="33"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -2486,7 +2681,7 @@
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="32" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -2495,21 +2690,21 @@
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="29"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="29"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="29"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
@@ -2519,6 +2714,7 @@
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2526,8 +2722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332F7ACA-D869-418F-9656-C9490FCFBDDB}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,56 +2744,56 @@
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="31"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="32"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
@@ -2671,7 +2867,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>31</v>
@@ -2888,6 +3084,7 @@
     <hyperlink ref="D20" r:id="rId9" xr:uid="{6464FCA1-8916-444E-91E6-F8AC00D2DB44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -2895,8 +3092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F22024E-17C1-41A8-A40B-9EDF611410C9}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,7 +3125,7 @@
       </c>
       <c r="J2" s="23">
         <f>COUNTIF(J7:J26, "Pass")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2955,7 +3152,7 @@
       </c>
       <c r="J5" s="23">
         <f>SUM(J2:J4)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="18" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3104,7 +3301,9 @@
       <c r="G10" s="12"/>
       <c r="H10" s="15"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="16"/>
+      <c r="J10" s="16" t="s">
+        <v>80</v>
+      </c>
       <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -3486,6 +3685,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3493,8 +3693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95C58AD-8E3C-4836-8664-CB0306E39F18}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="E25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3502,8 +3702,8 @@
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23" style="4" customWidth="1"/>
+    <col min="5" max="5" width="44.5703125" customWidth="1"/>
     <col min="6" max="6" width="45.85546875" customWidth="1"/>
     <col min="7" max="7" width="41.28515625" customWidth="1"/>
     <col min="8" max="8" width="45.85546875" customWidth="1"/>
@@ -3527,7 +3727,7 @@
       </c>
       <c r="K2" s="23">
         <f>COUNTIF(J7:J33, "Pass")</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3536,7 +3736,7 @@
       </c>
       <c r="K3" s="23">
         <f>COUNTIF(J7:J33, "Fail")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3557,7 +3757,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>135</v>
       </c>
@@ -3570,7 +3770,7 @@
       <c r="D6" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="26" t="s">
         <v>141</v>
       </c>
       <c r="F6" s="9" t="s">
@@ -3602,7 +3802,7 @@
       <c r="B7" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="12" t="s">
         <v>146</v>
       </c>
       <c r="D7" s="14" t="s">
@@ -3612,7 +3812,7 @@
         <v>77</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>183</v>
@@ -3621,10 +3821,10 @@
         <v>184</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="J7" s="40" t="s">
-        <v>80</v>
+        <v>240</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>136</v>
       </c>
       <c r="K7" s="14"/>
       <c r="L7" s="11"/>
@@ -3646,7 +3846,7 @@
         <v>77</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>185</v>
@@ -3655,9 +3855,9 @@
         <v>186</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="J8" s="40" t="s">
+        <v>232</v>
+      </c>
+      <c r="J8" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K8" s="14"/>
@@ -3689,9 +3889,9 @@
         <v>186</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="J9" s="40" t="s">
+        <v>232</v>
+      </c>
+      <c r="J9" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K9" s="14"/>
@@ -3723,9 +3923,9 @@
         <v>202</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="J10" s="40" t="s">
+        <v>232</v>
+      </c>
+      <c r="J10" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K10" s="14"/>
@@ -3757,9 +3957,9 @@
         <v>193</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="J11" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="J11" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K11" s="14"/>
@@ -3791,9 +3991,9 @@
         <v>184</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="J12" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="J12" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K12" s="14"/>
@@ -3827,7 +4027,7 @@
       <c r="I13" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="J13" s="40" t="s">
+      <c r="J13" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K13" s="14"/>
@@ -3859,9 +4059,9 @@
         <v>201</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="J14" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="J14" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K14" s="14"/>
@@ -3893,9 +4093,9 @@
         <v>202</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="J15" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="J15" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K15" s="14"/>
@@ -3927,9 +4127,9 @@
         <v>184</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="J16" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="J16" s="28" t="s">
         <v>136</v>
       </c>
       <c r="K16" s="14"/>
@@ -3961,9 +4161,9 @@
         <v>206</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="J17" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="J17" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K17" s="14"/>
@@ -3995,9 +4195,9 @@
         <v>184</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="J18" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="J18" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K18" s="14"/>
@@ -4029,9 +4229,9 @@
         <v>209</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="J19" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="J19" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K19" s="14"/>
@@ -4044,7 +4244,7 @@
       <c r="B20" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="30" t="s">
         <v>210</v>
       </c>
       <c r="D20" s="14" t="s">
@@ -4053,25 +4253,25 @@
       <c r="E20" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="12" t="s">
         <v>183</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="I20" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="J20" s="40" t="s">
+      <c r="I20" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="J20" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K20" s="14"/>
       <c r="L20" s="11"/>
     </row>
-    <row r="21" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>163</v>
       </c>
@@ -4087,60 +4287,60 @@
       <c r="E21" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="14" t="s">
         <v>192</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="I21" s="39" t="s">
+      <c r="I21" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="J21" s="40" t="s">
+      <c r="J21" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K21" s="14"/>
       <c r="L21" s="11"/>
     </row>
-    <row r="22" spans="1:12" s="35" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+    <row r="22" spans="1:12" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="39" t="s">
-        <v>220</v>
-      </c>
-      <c r="D22" s="38" t="s">
+      <c r="C22" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="I22" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="G22" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="H22" s="39" t="s">
-        <v>223</v>
-      </c>
-      <c r="I22" s="39" t="s">
-        <v>225</v>
-      </c>
-      <c r="J22" s="33" t="s">
+      <c r="J22" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="K22" s="38"/>
+      <c r="K22" s="14"/>
       <c r="L22" s="11"/>
     </row>
-    <row r="23" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+    <row r="23" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>165</v>
       </c>
       <c r="B23" s="14" t="s">
@@ -4155,26 +4355,26 @@
       <c r="E23" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="39" t="s">
-        <v>224</v>
-      </c>
-      <c r="G23" s="39" t="s">
+      <c r="F23" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>185</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="I23" s="39" t="s">
-        <v>222</v>
-      </c>
-      <c r="J23" s="40" t="s">
+        <v>218</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="J23" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K23" s="14"/>
       <c r="L23" s="11"/>
     </row>
     <row r="24" spans="1:12" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="14" t="s">
         <v>166</v>
       </c>
       <c r="B24" s="14" t="s">
@@ -4189,59 +4389,61 @@
       <c r="E24" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="39" t="s">
-        <v>229</v>
-      </c>
-      <c r="G24" s="39" t="s">
+      <c r="F24" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="G24" s="12" t="s">
         <v>183</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="J24" s="40" t="s">
+        <v>223</v>
+      </c>
+      <c r="J24" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K24" s="14"/>
       <c r="L24" s="11"/>
     </row>
-    <row r="25" spans="1:12" s="35" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="38" t="s">
+    <row r="25" spans="1:12" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="H25" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="I25" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="D25" s="38" t="s">
-        <v>169</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="F25" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="G25" s="38" t="s">
-        <v>192</v>
-      </c>
-      <c r="H25" s="37" t="s">
-        <v>231</v>
-      </c>
-      <c r="I25" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="J25" s="40" t="s">
+      <c r="J25" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="K25" s="38"/>
+      <c r="K25" s="14"/>
       <c r="L25" s="11"/>
     </row>
     <row r="26" spans="1:12" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
-        <v>167</v>
+      <c r="A26" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>144</v>
@@ -4255,27 +4457,27 @@
       <c r="E26" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="39" t="s">
-        <v>234</v>
-      </c>
-      <c r="G26" s="38" t="s">
+      <c r="F26" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="G26" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="H26" s="39" t="s">
+      <c r="H26" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="I26" s="39" t="s">
-        <v>235</v>
-      </c>
-      <c r="J26" s="40" t="s">
+      <c r="I26" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="J26" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K26" s="14"/>
       <c r="L26" s="11"/>
     </row>
     <row r="27" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
-        <v>168</v>
+      <c r="A27" s="14" t="s">
+        <v>174</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>144</v>
@@ -4290,26 +4492,26 @@
         <v>77</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="G27" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="H27" s="39" t="s">
+      <c r="H27" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="I27" s="39" t="s">
-        <v>235</v>
-      </c>
-      <c r="J27" s="40" t="s">
+      <c r="I27" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="J27" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K27" s="14"/>
       <c r="L27" s="11"/>
     </row>
     <row r="28" spans="1:12" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
-        <v>174</v>
+      <c r="A28" s="14" t="s">
+        <v>215</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>144</v>
@@ -4323,29 +4525,27 @@
       <c r="E28" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F28" s="34" t="s">
+      <c r="F28" s="29" t="s">
         <v>208</v>
       </c>
-      <c r="G28" s="38" t="s">
+      <c r="G28" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="H28" s="37" t="s">
-        <v>237</v>
-      </c>
-      <c r="I28" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="J28" s="40" t="s">
+      <c r="H28" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="I28" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="J28" s="31" t="s">
         <v>80</v>
       </c>
       <c r="K28" s="14"/>
       <c r="L28" s="11"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
-        <v>215</v>
-      </c>
-      <c r="B29" s="28"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="12"/>
       <c r="D29" s="14"/>
       <c r="E29" s="12"/>
@@ -4358,11 +4558,9 @@
       <c r="L29" s="11"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="36"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="14"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
@@ -4374,11 +4572,9 @@
       <c r="L30" s="11"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="36"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="14"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
@@ -4390,10 +4586,8 @@
       <c r="L31" s="11"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
-        <v>218</v>
-      </c>
-      <c r="B32" s="28"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="12"/>
       <c r="D32" s="14"/>
       <c r="E32" s="12"/>
@@ -4406,10 +4600,8 @@
       <c r="L32" s="11"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
-        <v>219</v>
-      </c>
-      <c r="B33" s="28"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="12"/>
       <c r="D33" s="14"/>
       <c r="E33" s="12"/>
@@ -4425,27 +4617,27 @@
       <c r="A34" s="14"/>
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
-      <c r="L34" s="26"/>
+      <c r="L34" s="25"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
-      <c r="L35" s="26"/>
+      <c r="L35" s="25"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J36" s="24"/>
       <c r="K36" s="24"/>
-      <c r="L36" s="26"/>
+      <c r="L36" s="25"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J37" s="24"/>
       <c r="K37" s="24"/>
-      <c r="L37" s="26"/>
+      <c r="L37" s="25"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J38" s="24"/>
       <c r="K38" s="24"/>
-      <c r="L38" s="26"/>
+      <c r="L38" s="25"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J39" s="24"/>
@@ -4455,17 +4647,493 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C782A2-E8A7-46DA-B5EE-2B2FA438DEC5}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="I1" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="I2" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="23">
+        <f>COUNTIF(J7:J14, "Pass")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="I3" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" s="23">
+        <f>COUNTIF(J7:J14, "Fail")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="I4" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="J4" s="23">
+        <f>COUNTIF(J7:J14, "Wrpmg")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="I5" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="J5" s="23">
+        <f>SUM(J2:J4)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="K8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" spans="1:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="14"/>
+    </row>
+    <row r="12" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>192</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="I14" s="39"/>
+      <c r="J14" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" s="39"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="45"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="40"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="40"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="40"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="40"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F13" r:id="rId1" xr:uid="{103A9710-6DF8-4C96-8D6E-C98870A02DCE}"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="46" fitToHeight="0" orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add add to cart functionality test
</commit_message>
<xml_diff>
--- a/Test Cases of pickaboo.com(Full & Final ).xlsx
+++ b/Test Cases of pickaboo.com(Full & Final ).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SQA2\Projects\Test Cases of pickaboo.com(Full &amp; Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8B4813-CE9E-4F10-80AA-1E5BB94CDE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D63A6D-B79B-420A-9D94-5166B18468C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="796" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="796" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="8" r:id="rId1"/>
@@ -19,10 +19,10 @@
     <sheet name="Login" sheetId="5" r:id="rId4"/>
     <sheet name="Logout" sheetId="6" r:id="rId5"/>
     <sheet name="Forgot Password" sheetId="14" r:id="rId6"/>
-    <sheet name="My Account" sheetId="17" r:id="rId7"/>
-    <sheet name="Change Password" sheetId="16" r:id="rId8"/>
-    <sheet name="Search" sheetId="13" r:id="rId9"/>
-    <sheet name="Add to Cart" sheetId="9" r:id="rId10"/>
+    <sheet name="Add to Cart" sheetId="9" r:id="rId7"/>
+    <sheet name="My Account" sheetId="17" r:id="rId8"/>
+    <sheet name="Change Password" sheetId="16" r:id="rId9"/>
+    <sheet name="Search" sheetId="13" r:id="rId10"/>
     <sheet name="Check Out" sheetId="15" r:id="rId11"/>
     <sheet name="Wishlist" sheetId="12" r:id="rId12"/>
     <sheet name="Template" sheetId="11" r:id="rId13"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="343">
   <si>
     <t>Project Name</t>
   </si>
@@ -2035,6 +2035,200 @@
   </si>
   <si>
     <t>https://www.pickaboo.com/</t>
+  </si>
+  <si>
+    <t>TC_ATC_001</t>
+  </si>
+  <si>
+    <t>(TS_006)
+Add to Cart</t>
+  </si>
+  <si>
+    <t>Verify adding the product to Cart from 'Wish List' Page</t>
+  </si>
+  <si>
+    <t>Verify adding the product to Cart from 'Product Display Page'</t>
+  </si>
+  <si>
+    <t>Verify adding the product to Cart from 'Search Result' Page</t>
+  </si>
+  <si>
+    <t>Verify the 'Add to Cart' page functionality in all the supported enviroments</t>
+  </si>
+  <si>
+    <t>Verify adding the product to Cart which product is not in Stock.</t>
+  </si>
+  <si>
+    <t>Add the same item multiple times and verify.</t>
+  </si>
+  <si>
+    <t>Verify adding multiple items of different types</t>
+  </si>
+  <si>
+    <t>TC_ATC_002</t>
+  </si>
+  <si>
+    <t>TC_ATC_003</t>
+  </si>
+  <si>
+    <t>TC_ATC_004</t>
+  </si>
+  <si>
+    <t>TC_ATC_005</t>
+  </si>
+  <si>
+    <t>TC_ATC_007</t>
+  </si>
+  <si>
+    <t>TC_ATC_008</t>
+  </si>
+  <si>
+    <t>TC_ATC_009</t>
+  </si>
+  <si>
+    <t>TC_ATC_010</t>
+  </si>
+  <si>
+    <t>TC_ATC_011</t>
+  </si>
+  <si>
+    <t>TC_ATC_012</t>
+  </si>
+  <si>
+    <t>Add item(s) to the cart, close the browser and reopen the same site.</t>
+  </si>
+  <si>
+    <t>Remove some items from the cart and verify</t>
+  </si>
+  <si>
+    <t>Remove all items from the cart and then verify.</t>
+  </si>
+  <si>
+    <t>Click on an item in the cart and verify that the user is redirected to the product detail page.</t>
+  </si>
+  <si>
+    <t>TC_ATC_013</t>
+  </si>
+  <si>
+    <t>TC_ATC_014</t>
+  </si>
+  <si>
+    <t>1. Open the application and login.</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into he Search Tex Box field.
+2. Click on the button having search results. 
+3. Click on the Product displayed in the Search results
+4. Click on 'Add to Cart' button in the displa yed Product page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Success massage with text ' You added Samsung F23(83878) to your shopping cart.
+2. Product should be display in the ' Cart' page </t>
+  </si>
+  <si>
+    <t>1. Product should not add in the 'Cart' again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the application and login.
+</t>
+  </si>
+  <si>
+    <t>1. Click on 'Cart' menu 
+2. Select 'Wish List' dropdown menu and click.
+3. Click on the product.
+4. Add to cart.</t>
+  </si>
+  <si>
+    <t>Product Name: Samsung Galaxy F23</t>
+  </si>
+  <si>
+    <t>Verify adding the product to Cart from the Similar products section of the Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Click on the any Product
+2. Go to 'Product Display' page
+4. Scroll down on the page and check 'Similar product'
+5. Click on the product.
+6. Click on 'Add to Cart' option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Success massage with text ' You added (Product Name) to your shopping cart.
+2. Product should be display in the ' Cart' page </t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into he Search Tex Box field.
+2. Click on the button having search results. 
+3. Click on the Product displayed in the Search results
+4. Click on 'Add to Cart' button in the displayed Product page.</t>
+  </si>
+  <si>
+    <t>1. Click on the any Product
+2. Go to 'Product Display' page
+3. Click on 'Add to Cart' button in the displayed Product page
+4. Click on again ' Add to Cart' button.</t>
+  </si>
+  <si>
+    <t>1. Warning massage with text' Product is alredy on your cart'</t>
+  </si>
+  <si>
+    <t>Product Name: 
+1. Mi Beard Trimmer IPX7</t>
+  </si>
+  <si>
+    <t>Product Name: 
+1. Mi Beard Trimmer IPX7
+2. Fastrack 3192AL01 
+3. Panasonic</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into he Search Tex Box field.
+2. Click on the button having search results. Click on the any Product
+3. Go to 'Product Display' page
+4. Click on 'Add to Cart' button in the displayed Product page
+5. Repet the step 1, 2 , 3 and 4
+6. adding multiple product on 'Cart'</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into he Search Tex Box field.
+2. Click on the button having search results. 
+3. Click on the Product displayed in the Search results
+4. Close the browser 
+5. Again open the browser and open the application
+6. Check the 'Cart' page that items are sitll added.</t>
+  </si>
+  <si>
+    <t>1. Product should not be remove in the 'Cart' page.</t>
+  </si>
+  <si>
+    <t>1. All products should be ad  in the 'Cart' page.</t>
+  </si>
+  <si>
+    <t>1. Products should be removing from 'Cart' page</t>
+  </si>
+  <si>
+    <t>1. Open 'Cart' menu 
+2. Removeing some items from cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the application and login.
+2. Producs should add on 'Cart' </t>
+  </si>
+  <si>
+    <t>1. All products should be removing from 'Cart' page</t>
+  </si>
+  <si>
+    <t>1. Open 'Cart' menu 
+2. Removeing all items from cart</t>
+  </si>
+  <si>
+    <t>1. Open 'Cart' manu
+2. Click on any product</t>
+  </si>
+  <si>
+    <t>1. Page should be redirected to the product detail page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2723,11 +2917,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B02E6E-466D-46E8-9EC5-97DD2A519152}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9398FE18-F224-4C16-9E97-ECD2DB8B161A}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4182,8 +4376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332F7ACA-D869-418F-9656-C9490FCFBDDB}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5153,7 +5347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95C58AD-8E3C-4836-8664-CB0306E39F18}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="E7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -6118,7 +6312,7 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -6557,7 +6751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1D6D1D-D934-49DC-940E-1A93D2F5E2D1}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -6918,6 +7112,619 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B02E6E-466D-46E8-9EC5-97DD2A519152}">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="44.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="41" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="I1" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="I2" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="23">
+        <f>COUNTIF(J7:J20, "Pass")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="I3" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" s="23">
+        <f>COUNTIF(J7:J20, "Fail")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="I4" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="J4" s="23">
+        <f>COUNTIF(J7:J20, "Wrpmg")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="I5" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="J5" s="23">
+        <f>SUM(J2:J4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="H17" s="12"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="12"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94942F9E-45C7-4B29-83B5-1A2A1569DC17}">
   <dimension ref="A1:K25"/>
   <sheetViews>
@@ -7281,7 +8088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7B2B6D-3C64-421F-9490-B9AE76834FBF}">
   <dimension ref="A1:K25"/>
   <sheetViews>
@@ -7643,368 +8450,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9398FE18-F224-4C16-9E97-ECD2DB8B161A}">
-  <dimension ref="A1:K25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="I1" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="I2" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="23">
-        <f>COUNTIF(J7:J14, "Pass")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="I3" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="J3" s="23">
-        <f>COUNTIF(J7:J14, "Fail")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="I4" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="J4" s="23">
-        <f>COUNTIF(J7:J14, "Wrpmg")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="I5" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="J5" s="23">
-        <f>SUM(J2:J4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="12"/>
-    </row>
-    <row r="8" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12"/>
-    </row>
-    <row r="13" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="12"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="12"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="12"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="12"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="12"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="12"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="12"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update add to cart funcionality testing
</commit_message>
<xml_diff>
--- a/Test Cases of pickaboo.com(Full & Final ).xlsx
+++ b/Test Cases of pickaboo.com(Full & Final ).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SQA2\Projects\Test Cases of pickaboo.com(Full &amp; Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D63A6D-B79B-420A-9D94-5166B18468C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF86555D-A741-4140-863A-2A7A9EF21D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="796" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="358">
   <si>
     <t>Project Name</t>
   </si>
@@ -2110,9 +2110,6 @@
     <t>TC_ATC_013</t>
   </si>
   <si>
-    <t>TC_ATC_014</t>
-  </si>
-  <si>
     <t>1. Open the application and login.</t>
   </si>
   <si>
@@ -2200,9 +2197,6 @@
     <t>1. Product should not be remove in the 'Cart' page.</t>
   </si>
   <si>
-    <t>1. All products should be ad  in the 'Cart' page.</t>
-  </si>
-  <si>
     <t>1. Products should be removing from 'Cart' page</t>
   </si>
   <si>
@@ -2228,7 +2222,63 @@
     <t>1. Page should be redirected to the product detail page</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>1. Enter any existing product name into he Search Tex Box field.
+2. Click on the button having search results. 
+3. Click on the Product displayed in the Search results
+4. Click on 'Add to Cart' button</t>
+  </si>
+  <si>
+    <t>Product Name: Xaomi note 8</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL in any supported browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Check the 'Add to Cart' functionality in all the supported environments </t>
+  </si>
+  <si>
+    <t>1. 'Add to Cart' functionality should work correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t>TC_ATC_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Get success massage with text ' You added Samsung F23(83878) to your shopping cart.
+2. Product is display in the 'Cart' page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Success massage with text ' You added Samsung F23(83878) to your shopping cart.
+2. Product should be display in the 'Cart' page </t>
+  </si>
+  <si>
+    <t>1. Product is not add in the 'Cart' again.</t>
+  </si>
+  <si>
+    <t>1.Get success massage with text ' You added Samsung F23(83878) to your shopping cart.</t>
+  </si>
+  <si>
+    <t>1. All products is added  in the 'Cart' page.</t>
+  </si>
+  <si>
+    <t>1. All products should be add  in the 'Cart' page.</t>
+  </si>
+  <si>
+    <t>1. Product is  not be remove in the 'Cart' page.</t>
+  </si>
+  <si>
+    <t>1. No option to add on Cart</t>
+  </si>
+  <si>
+    <t>1. All products are removing from 'Cart' page</t>
+  </si>
+  <si>
+    <t>1. Products are remove from 'Cart' page</t>
+  </si>
+  <si>
+    <t>1. Page is redirected to the product detail page</t>
+  </si>
+  <si>
+    <t>1. 'Add to Cart' functionality is work correctly in all the supported environments</t>
   </si>
 </sst>
 </file>
@@ -6313,7 +6363,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7115,8 +7165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B02E6E-466D-46E8-9EC5-97DD2A519152}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7128,9 +7178,9 @@
     <col min="5" max="5" width="44.5703125" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" customWidth="1"/>
     <col min="7" max="7" width="41" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" customWidth="1"/>
     <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
     <col min="11" max="11" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7152,7 +7202,7 @@
       </c>
       <c r="J2" s="23">
         <f>COUNTIF(J7:J20, "Pass")</f>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7163,7 +7213,7 @@
       </c>
       <c r="J3" s="23">
         <f>COUNTIF(J7:J20, "Fail")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7185,7 +7235,7 @@
       </c>
       <c r="J5" s="23">
         <f>SUM(J2:J4)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7234,20 +7284,24 @@
         <v>294</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="H7" s="12"/>
+        <v>347</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>346</v>
+      </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="J7" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7261,20 +7315,24 @@
         <v>298</v>
       </c>
       <c r="D8" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>317</v>
-      </c>
       <c r="F8" s="12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="H8" s="12"/>
+        <v>318</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>348</v>
+      </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="J8" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:11" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7288,20 +7346,24 @@
         <v>293</v>
       </c>
       <c r="D9" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="F9" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>322</v>
-      </c>
       <c r="G9" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="H9" s="12"/>
+        <v>317</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>346</v>
+      </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:11" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7315,20 +7377,22 @@
         <v>295</v>
       </c>
       <c r="D10" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="F10" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>317</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>318</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="J10" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7339,28 +7403,30 @@
         <v>292</v>
       </c>
       <c r="C11" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>323</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>324</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>192</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="J11" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:11" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>304</v>
+        <v>345</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>292</v>
@@ -7369,25 +7435,29 @@
         <v>298</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>192</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="H12" s="12"/>
+        <v>327</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>349</v>
+      </c>
       <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="J12" s="40" t="s">
+        <v>136</v>
+      </c>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>292</v>
@@ -7396,25 +7466,29 @@
         <v>299</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="H13" s="12"/>
+        <v>351</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>350</v>
+      </c>
       <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="J13" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>292</v>
@@ -7423,25 +7497,29 @@
         <v>310</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E14" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="F14" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="H14" s="12"/>
+      <c r="H14" s="12" t="s">
+        <v>352</v>
+      </c>
       <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="J14" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>292</v>
@@ -7450,25 +7528,29 @@
         <v>311</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>192</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="H15" s="12"/>
+        <v>333</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>355</v>
+      </c>
       <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="J15" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>292</v>
@@ -7477,25 +7559,29 @@
         <v>312</v>
       </c>
       <c r="D16" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>337</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>339</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>192</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="H16" s="12"/>
+        <v>336</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>354</v>
+      </c>
       <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+      <c r="J16" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>292</v>
@@ -7504,25 +7590,29 @@
         <v>313</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>192</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="H17" s="12"/>
+        <v>339</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>356</v>
+      </c>
       <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="J17" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>292</v>
@@ -7531,21 +7621,29 @@
         <v>297</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
+        <v>340</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>353</v>
+      </c>
       <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+      <c r="J18" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>292</v>
@@ -7553,13 +7651,25 @@
       <c r="C19" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
+      <c r="D19" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>343</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>344</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>357</v>
+      </c>
       <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
+      <c r="J19" s="41" t="s">
+        <v>80</v>
+      </c>
       <c r="K19" s="12"/>
     </row>
     <row r="20" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Write Product Details Testcase
</commit_message>
<xml_diff>
--- a/Test Cases of pickaboo.com(Full & Final ).xlsx
+++ b/Test Cases of pickaboo.com(Full & Final ).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SQA2\Projects\Test Cases of pickaboo.com(Full &amp; Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF86555D-A741-4140-863A-2A7A9EF21D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3021C13-53AD-43E8-959A-3E32B66639BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="796" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="796" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="8" r:id="rId1"/>
@@ -20,12 +20,13 @@
     <sheet name="Logout" sheetId="6" r:id="rId5"/>
     <sheet name="Forgot Password" sheetId="14" r:id="rId6"/>
     <sheet name="Add to Cart" sheetId="9" r:id="rId7"/>
-    <sheet name="My Account" sheetId="17" r:id="rId8"/>
-    <sheet name="Change Password" sheetId="16" r:id="rId9"/>
-    <sheet name="Search" sheetId="13" r:id="rId10"/>
-    <sheet name="Check Out" sheetId="15" r:id="rId11"/>
-    <sheet name="Wishlist" sheetId="12" r:id="rId12"/>
-    <sheet name="Template" sheetId="11" r:id="rId13"/>
+    <sheet name="Product Details" sheetId="18" r:id="rId8"/>
+    <sheet name="My Account" sheetId="17" r:id="rId9"/>
+    <sheet name="Change Password" sheetId="16" r:id="rId10"/>
+    <sheet name="Search" sheetId="13" r:id="rId11"/>
+    <sheet name="Check Out" sheetId="15" r:id="rId12"/>
+    <sheet name="Wishlist" sheetId="12" r:id="rId13"/>
+    <sheet name="Template" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="424">
   <si>
     <t>Project Name</t>
   </si>
@@ -2279,6 +2280,419 @@
   </si>
   <si>
     <t>1. 'Add to Cart' functionality is work correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t>TC_PD_001</t>
+  </si>
+  <si>
+    <t>TS_007
+Product Details</t>
+  </si>
+  <si>
+    <t>Verfiy the Thumbnails of the product displayed in the product display page</t>
+  </si>
+  <si>
+    <t>TC_PD_002</t>
+  </si>
+  <si>
+    <t>TC_PD_003</t>
+  </si>
+  <si>
+    <t>TC_PD_004</t>
+  </si>
+  <si>
+    <t>TC_PD_005</t>
+  </si>
+  <si>
+    <t>TC_PD_006</t>
+  </si>
+  <si>
+    <t>TC_PD_007</t>
+  </si>
+  <si>
+    <t>TC_PD_008</t>
+  </si>
+  <si>
+    <t>TC_PD_009</t>
+  </si>
+  <si>
+    <t>TC_PD_010</t>
+  </si>
+  <si>
+    <t>TC_PD_011</t>
+  </si>
+  <si>
+    <t>TC_PD_012</t>
+  </si>
+  <si>
+    <t>TC_PD_013</t>
+  </si>
+  <si>
+    <t>TC_PD_014</t>
+  </si>
+  <si>
+    <t>TC_PD_015</t>
+  </si>
+  <si>
+    <t>TC_PD_016</t>
+  </si>
+  <si>
+    <t>TC_PD_017</t>
+  </si>
+  <si>
+    <t>TC_PD_018</t>
+  </si>
+  <si>
+    <t>TC_PD_019</t>
+  </si>
+  <si>
+    <t>Verify the availablity status of the Produc Details Page</t>
+  </si>
+  <si>
+    <t>Verify that Product Name, Brand and Product Code re displayed in the Product Details Page</t>
+  </si>
+  <si>
+    <t>Vefiry the Price of the Product with and without tax is displayed in the Product Display Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify the default quantity for the Product is displayed as 1 in the Product Display Page, When there is no minimum quantity set for the Product </t>
+  </si>
+  <si>
+    <t>Verfiy the negative quantity or zero quantity or null quantity should not be allowed in the Product Details Page</t>
+  </si>
+  <si>
+    <t>Vefiry the Product having the minimum quantity set</t>
+  </si>
+  <si>
+    <t>Verify the User is able to write a review for the Product form the 'Reviews' tab of Product Details Page</t>
+  </si>
+  <si>
+    <t>Verify the 'Reviews' tab when there are no reviews or zero reviews added</t>
+  </si>
+  <si>
+    <t>Verify 'Write a review' link under 'Add to Cart' button on the Product Details Page</t>
+  </si>
+  <si>
+    <t>Verify the count of reviews should be displayed int 'Reviews' tab label of the Product Details Page</t>
+  </si>
+  <si>
+    <t>Verify 'reviews' link under the 'Add to Cart' button of Product Display Page</t>
+  </si>
+  <si>
+    <t>Verify submitting a review without filling the mandatory fields</t>
+  </si>
+  <si>
+    <t>Verify the review text given while writing is accepted according to the secified number of characters.</t>
+  </si>
+  <si>
+    <t>Verify adding the Product to 'Wish List' from the Product Details Page</t>
+  </si>
+  <si>
+    <t>Verify Product for comparision from the Product Details Page</t>
+  </si>
+  <si>
+    <t>Verify proper option for linking, tweeting, sharing the Product Display page on social  platfroms</t>
+  </si>
+  <si>
+    <t>Verify 'Related Products' Section in Product Details Page</t>
+  </si>
+  <si>
+    <t>TC_PD_020</t>
+  </si>
+  <si>
+    <t>TC_PD_021</t>
+  </si>
+  <si>
+    <t>TC_PD_022</t>
+  </si>
+  <si>
+    <t>TC_PD_023</t>
+  </si>
+  <si>
+    <t>TC_PD_024</t>
+  </si>
+  <si>
+    <t>TC_PD_025</t>
+  </si>
+  <si>
+    <t>TC_PD_026</t>
+  </si>
+  <si>
+    <t>TC_PD_027</t>
+  </si>
+  <si>
+    <r>
+      <t>Verify navigating to the Product Details Page by using the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Product Name Link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">'Wish List' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify navigating to the Product Details Page by using the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Product image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Wish List'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Verify navigating to the Product Details page by using the Product</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Shopping Cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Verify navigating to the Product Details page by using the Product</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Name link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Shopping Cart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' page</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify the Reward Points displayed in the Product Details Page</t>
+  </si>
+  <si>
+    <t>Verify the original price of the Product without offer in the Product Details Page</t>
+  </si>
+  <si>
+    <t>Verify Page Title , Page Heading and Page URL of the Product Details Page</t>
+  </si>
+  <si>
+    <t>Verify the 'Product Display' page functionality in all the supported environments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter any existing product name into the Search text box field
+2. Click on button having serarch icon
+3. Click on the Product Details in the Search result
+4. Click on the main bigger sized Thumbnail image displayed on the 'Product Details Page'
+5. Click on "&lt; and &gt;" option
+6. click on x (Close)  option or press 'ESC' keyboard key when the thumbnails are displayed in light box view 
+7. Click on the normal sized Thumbnail images and repeat the steps 5 to 6 </t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the Search text box field
+2. Click on button having serarch icon
+3. Click on the Product Details in the Search result
+4. Check the Product Name, Brand and Product  Code in the displayed Product Details Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the Search text box field
+2. Click on button having serarch icon
+3. Click on the Product Details in the Search result
+4. Check the different availability status of the Products in the displayed Product Details Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the Search text box field
+2. Click on button having serarch icon
+3. Click on the Product Details in the Search result
+4. Check the Price with Tax and Price Ex Tax in the displayed Product Details Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the Search text box field
+2. Click on button having serarch icon
+3. Click on the Product Details in the Search result
+4. Check the Qty text field in the Product Details Page 
+5. Update the Quantity in the Qty text field by providing a negative number or zero number or null quantity and click on 'Add to Cart' button</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the Search text box field
+2. Click on button having serarch icon
+3. Click on the Product Details in the Search result
+4. Check the Qty text field in the Product Details Page 
+5. Update the quantity by incressing it to more than one and click 'Add to Cart' Button</t>
+  </si>
+  <si>
+    <t>Verify the description of the Product in the Product Details Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the Search text box field
+2. Click on button having serarch icon
+3. Click on the Product Details in the Search result
+4. Click on the Description tab of the Prodcut in the displayed 'Product Details Page'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter any existing product name into the Search text box field
+2. Click on button having serarch icon
+3. Click on the Product Details in the Search result
+4. Click on the Review tab of the Product Details Page 
+5. Enter your name into the 'Your Name' text field 6. Enter review text int the 'Yur Review' text are field 
+7. Select any radio button to give the rating 
+8. Click on 'Continue' Button </t>
+  </si>
+  <si>
+    <t>Verify all the fields in the 'Review' tab are mandatory fields</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the Search text box field
+2. Click on button having serarch icon
+3. Click on the Product Details in the Search result
+4. Click on the Reviews tab of the Product in the display page and check</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the Search text box field
+2. Click on button having serarch icon
+3. Click on the Product Details in the Search result
+4.</t>
   </si>
 </sst>
 </file>
@@ -2967,6 +3381,371 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7B2B6D-3C64-421F-9490-B9AE76834FBF}">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="I1" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="I2" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="23">
+        <f>COUNTIF(J7:J14, "Pass")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="I3" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" s="23">
+        <f>COUNTIF(J7:J14, "Fail")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="I4" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="J4" s="23">
+        <f>COUNTIF(J7:J14, "Wrpmg")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="I5" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="J5" s="23">
+        <f>SUM(J2:J4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9398FE18-F224-4C16-9E97-ECD2DB8B161A}">
   <dimension ref="A1:K25"/>
   <sheetViews>
@@ -3327,10 +4106,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7D98CC-E497-4A2F-A05A-818A027F4FCE}">
   <dimension ref="A1:K25"/>
   <sheetViews>
@@ -3691,10 +4471,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CBA276-A102-4D64-A77F-25781A61F136}">
   <dimension ref="A1:K25"/>
   <sheetViews>
@@ -4055,10 +4836,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2A6343-3B72-4494-964E-5F61599E5A50}">
   <dimension ref="A1:K25"/>
   <sheetViews>
@@ -4419,6 +5201,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4426,7 +5209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332F7ACA-D869-418F-9656-C9490FCFBDDB}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -4797,7 +5580,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A7" sqref="A7:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5397,7 +6180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95C58AD-8E3C-4836-8664-CB0306E39F18}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="E25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -6362,7 +7145,7 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -7158,6 +7941,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7165,7 +7949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B02E6E-466D-46E8-9EC5-97DD2A519152}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -7831,10 +8615,780 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B83402-9CF4-4B99-AD26-2570C909472C}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="I1" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="I2" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="23">
+        <f>COUNTIF(J7:J14, "Pass")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="I3" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" s="23">
+        <f>COUNTIF(J7:J14, "Fail")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="I4" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="J4" s="23">
+        <f>COUNTIF(J7:J14, "Wrpmg")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="I5" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="J5" s="23">
+        <f>SUM(J2:J4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="225" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" ht="183" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>405</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="12"/>
+    </row>
+    <row r="32" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>400</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="12"/>
+    </row>
+    <row r="33" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="12"/>
+    </row>
+    <row r="34" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="12"/>
+    </row>
+    <row r="35" spans="1:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>411</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="12"/>
+    </row>
+    <row r="36" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="10" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94942F9E-45C7-4B29-83B5-1A2A1569DC17}">
   <dimension ref="A1:K25"/>
   <sheetViews>
@@ -8195,369 +9749,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7B2B6D-3C64-421F-9490-B9AE76834FBF}">
-  <dimension ref="A1:K25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="I1" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="I2" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="23">
-        <f>COUNTIF(J7:J14, "Pass")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="I3" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="J3" s="23">
-        <f>COUNTIF(J7:J14, "Fail")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="I4" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="J4" s="23">
-        <f>COUNTIF(J7:J14, "Wrpmg")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="I5" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="J5" s="23">
-        <f>SUM(J2:J4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="12"/>
-    </row>
-    <row r="8" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12"/>
-    </row>
-    <row r="13" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="12"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="12"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="12"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="12"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="12"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="12"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="12"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Product Details Page Functionality Test are done
</commit_message>
<xml_diff>
--- a/Test Cases of pickaboo.com(Full & Final ).xlsx
+++ b/Test Cases of pickaboo.com(Full & Final ).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SQA2\Projects\Test Cases of pickaboo.com(Full &amp; Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F626C8-24EE-4F3A-951D-1DE15F77C910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4832FFDF-3978-41C1-B80D-2168BDE41089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="796" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="796" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="502">
   <si>
     <t>Project Name</t>
   </si>
@@ -2896,10 +2896,6 @@
 5. Back to Product Details Page and click on 'Add to Cart' check</t>
   </si>
   <si>
-    <t xml:space="preserve">1. When click on 'Buy Now', page will be redirect to Cart option. 
-2. When Clik on 'Add to Cart', page will be redirect to Cart option. </t>
-  </si>
-  <si>
     <t>Verify the Sold by link will be redirect to Seller Page.</t>
   </si>
   <si>
@@ -3071,6 +3067,104 @@
   </si>
   <si>
     <t xml:space="preserve">Product Name: Apple MacBook </t>
+  </si>
+  <si>
+    <t>1. Thumbnail is display and  zoom able</t>
+  </si>
+  <si>
+    <t>1. All images are displaye visible properly</t>
+  </si>
+  <si>
+    <t>1. Name, Brand , Sold By, Vlub Points field are set on actual place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Color option is selectable </t>
+  </si>
+  <si>
+    <t>1. Main price, Orginal price and Discount are showing displayed Product Details Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Minimum quantity is one and can  be incress value for the Product </t>
+  </si>
+  <si>
+    <t>1. Negative quantity or zero quantity or null quantity is notbe setable</t>
+  </si>
+  <si>
+    <t>1. The Product having the minimum quantity set '1'</t>
+  </si>
+  <si>
+    <t>1. Product description is showing on Product Details Page</t>
+  </si>
+  <si>
+    <t>1. Review is not showing on Product Detail Page</t>
+  </si>
+  <si>
+    <t>1. Total Review and Avarage Ratting are visible properly</t>
+  </si>
+  <si>
+    <t>Verify Review like dislike can be work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter any existing product name into the Search text box field
+2. Click on button having serarch icon
+3. Click on the Product Details in the Search result
+4. Click on like or dislike button </t>
+  </si>
+  <si>
+    <t>1. User should be able to Like or Dislike the review</t>
+  </si>
+  <si>
+    <t>1. User is not  able to Like or Dislike the review</t>
+  </si>
+  <si>
+    <t>1. User are able to write Product title, description and select rating properly but not submitable</t>
+  </si>
+  <si>
+    <t>1. Review Page is showng as a pop up page</t>
+  </si>
+  <si>
+    <t>1. All revieware showing in the Product Details Page</t>
+  </si>
+  <si>
+    <t>1. All review are showing Less number of review in the Product Details Page</t>
+  </si>
+  <si>
+    <t>1. Button is not work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. When click on 'Buy Now', page will be redirect to Cart option. 
+2. When Click on 'Add to Cart', page will be Success massage with text ' You added (Product Name) to your shopping cart.' </t>
+  </si>
+  <si>
+    <t>1. 'Buy Now', page is redirect to Cart option. 
+2.  'Add to Cart' button is not working for some product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Some product is not add on Cart option, Ex 'Infinix Smart 7 X6515 4GB/64GB' </t>
+  </si>
+  <si>
+    <t>1.Link is redirect to seller products page</t>
+  </si>
+  <si>
+    <t>1. Display pop up page for EMI details with Bank Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Imgages are not visible properly </t>
+  </si>
+  <si>
+    <t>1. Product is shareable on Social Media timeline</t>
+  </si>
+  <si>
+    <t>1. Product is redirect to Product Details Page</t>
+  </si>
+  <si>
+    <t>1. Orignal price is displayed as striked off</t>
+  </si>
+  <si>
+    <t>1. 'Product  Details' page functionality are work correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t>TC_PD_030</t>
   </si>
 </sst>
 </file>
@@ -3270,7 +3364,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3395,6 +3489,12 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3406,18 +3506,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3716,10 +3804,10 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="43"/>
+      <c r="C6" s="45"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -3740,7 +3828,7 @@
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="44" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -3749,17 +3837,17 @@
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="42"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
+      <c r="B12" s="44"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
@@ -3777,7 +3865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7B2B6D-3C64-421F-9490-B9AE76834FBF}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -4142,7 +4230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9398FE18-F224-4C16-9E97-ECD2DB8B161A}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -4507,7 +4595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7D98CC-E497-4A2F-A05A-818A027F4FCE}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -4872,7 +4960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CBA276-A102-4D64-A77F-25781A61F136}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -5237,7 +5325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2A6343-3B72-4494-964E-5F61599E5A50}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -5602,7 +5690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332F7ACA-D869-418F-9656-C9490FCFBDDB}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -5624,56 +5712,56 @@
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="44"/>
+      <c r="E2" s="46"/>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="45"/>
+      <c r="E3" s="47"/>
     </row>
     <row r="4" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
     </row>
     <row r="5" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="46"/>
     </row>
     <row r="6" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="44"/>
+      <c r="E6" s="46"/>
     </row>
     <row r="7" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
@@ -5972,7 +6060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F22024E-17C1-41A8-A40B-9EDF611410C9}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -6573,7 +6661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95C58AD-8E3C-4836-8664-CB0306E39F18}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -7538,8 +7626,8 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7977,7 +8065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1D6D1D-D934-49DC-940E-1A93D2F5E2D1}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -8342,8 +8430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B02E6E-466D-46E8-9EC5-97DD2A519152}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9017,10 +9105,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9055,8 +9143,8 @@
         <v>78</v>
       </c>
       <c r="J2" s="23">
-        <f>COUNTIF(J7:J15, "Pass")</f>
-        <v>0</v>
+        <f>COUNTIF(J7:J36, "Pass")</f>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9066,8 +9154,8 @@
         <v>134</v>
       </c>
       <c r="J3" s="23">
-        <f>COUNTIF(J7:J15, "Fail")</f>
-        <v>0</v>
+        <f>COUNTIF(J7:J36, "Fail")</f>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9089,7 +9177,7 @@
       </c>
       <c r="J5" s="23">
         <f>SUM(J2:J4)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9134,7 +9222,7 @@
       <c r="B7" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="12" t="s">
         <v>358</v>
       </c>
       <c r="D7" s="30" t="s">
@@ -9144,14 +9232,18 @@
         <v>419</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>420</v>
       </c>
-      <c r="H7" s="12"/>
+      <c r="H7" s="12" t="s">
+        <v>471</v>
+      </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="J7" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.25">
@@ -9161,24 +9253,28 @@
       <c r="B8" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C8" s="48" t="s">
-        <v>442</v>
+      <c r="C8" s="12" t="s">
+        <v>441</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>340</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>466</v>
-      </c>
-      <c r="H8" s="12"/>
+        <v>465</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>472</v>
+      </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="31"/>
+      <c r="J8" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:11" ht="114" customHeight="1" x14ac:dyDescent="0.25">
@@ -9188,7 +9284,7 @@
       <c r="B9" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="12" t="s">
         <v>422</v>
       </c>
       <c r="D9" s="30" t="s">
@@ -9198,14 +9294,18 @@
         <v>423</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>467</v>
-      </c>
-      <c r="H9" s="12"/>
+        <v>466</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>473</v>
+      </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:11" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9215,7 +9315,7 @@
       <c r="B10" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="12" t="s">
         <v>424</v>
       </c>
       <c r="D10" s="30" t="s">
@@ -9225,14 +9325,18 @@
         <v>425</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="H10" s="12"/>
+      <c r="H10" s="12" t="s">
+        <v>474</v>
+      </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="J10" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9242,7 +9346,7 @@
       <c r="B11" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="12" t="s">
         <v>427</v>
       </c>
       <c r="D11" s="30" t="s">
@@ -9252,14 +9356,18 @@
         <v>428</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>429</v>
       </c>
-      <c r="H11" s="12"/>
+      <c r="H11" s="12" t="s">
+        <v>475</v>
+      </c>
       <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="J11" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.25">
@@ -9269,7 +9377,7 @@
       <c r="B12" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="12" t="s">
         <v>377</v>
       </c>
       <c r="D12" s="30" t="s">
@@ -9279,14 +9387,18 @@
         <v>430</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>431</v>
       </c>
-      <c r="H12" s="12"/>
+      <c r="H12" s="12" t="s">
+        <v>476</v>
+      </c>
       <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="J12" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:11" ht="138" customHeight="1" x14ac:dyDescent="0.25">
@@ -9296,7 +9408,7 @@
       <c r="B13" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="12" t="s">
         <v>378</v>
       </c>
       <c r="D13" s="30" t="s">
@@ -9306,14 +9418,18 @@
         <v>395</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>468</v>
-      </c>
-      <c r="H13" s="12"/>
+        <v>467</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>477</v>
+      </c>
       <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="J13" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:11" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9323,7 +9439,7 @@
       <c r="B14" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="12" t="s">
         <v>416</v>
       </c>
       <c r="D14" s="30" t="s">
@@ -9333,14 +9449,18 @@
         <v>417</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="H14" s="12"/>
+      <c r="H14" s="12" t="s">
+        <v>478</v>
+      </c>
       <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="J14" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:11" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9350,7 +9470,7 @@
       <c r="B15" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="12" t="s">
         <v>396</v>
       </c>
       <c r="D15" s="30" t="s">
@@ -9360,14 +9480,18 @@
         <v>414</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="H15" s="12"/>
+      <c r="H15" s="12" t="s">
+        <v>479</v>
+      </c>
       <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="J15" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:11" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9377,7 +9501,7 @@
       <c r="B16" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="12" t="s">
         <v>400</v>
       </c>
       <c r="D16" s="30" t="s">
@@ -9387,15 +9511,21 @@
         <v>401</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>469</v>
-      </c>
-      <c r="H16" s="12"/>
+        <v>468</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>486</v>
+      </c>
       <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="12"/>
+      <c r="J16" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="17" spans="1:11" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
@@ -9404,7 +9534,7 @@
       <c r="B17" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="12" t="s">
         <v>397</v>
       </c>
       <c r="D17" s="30" t="s">
@@ -9414,177 +9544,207 @@
         <v>398</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>470</v>
-      </c>
-      <c r="H17" s="12"/>
+        <v>469</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>481</v>
+      </c>
       <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="J17" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>369</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="C18" s="48" t="s">
-        <v>379</v>
+      <c r="B18" s="14"/>
+      <c r="C18" s="12" t="s">
+        <v>482</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>407</v>
+        <v>340</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>402</v>
+        <v>483</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>403</v>
-      </c>
-      <c r="H18" s="12"/>
+        <v>484</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>485</v>
+      </c>
       <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="12"/>
-    </row>
-    <row r="19" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>370</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C19" s="48" t="s">
-        <v>411</v>
+      <c r="C19" s="12" t="s">
+        <v>379</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>407</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>413</v>
-      </c>
-      <c r="H19" s="12"/>
+        <v>403</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>403</v>
+      </c>
       <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
+      <c r="J19" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K19" s="12"/>
     </row>
-    <row r="20" spans="1:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>371</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C20" s="48" t="s">
-        <v>405</v>
+      <c r="C20" s="12" t="s">
+        <v>411</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>407</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>404</v>
-      </c>
-      <c r="H20" s="12"/>
+        <v>413</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>487</v>
+      </c>
       <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
+      <c r="J20" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K20" s="12"/>
     </row>
-    <row r="21" spans="1:11" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>372</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C21" s="48" t="s">
-        <v>408</v>
+      <c r="C21" s="12" t="s">
+        <v>405</v>
       </c>
       <c r="D21" s="30" t="s">
         <v>407</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>410</v>
-      </c>
-      <c r="H21" s="12"/>
+        <v>404</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>488</v>
+      </c>
       <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+      <c r="J21" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K21" s="12"/>
     </row>
-    <row r="22" spans="1:11" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>373</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C22" s="48" t="s">
-        <v>432</v>
+      <c r="C22" s="12" t="s">
+        <v>408</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>340</v>
+        <v>407</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>434</v>
-      </c>
-      <c r="H22" s="12"/>
+        <v>410</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>489</v>
+      </c>
       <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="J22" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K22" s="12"/>
     </row>
-    <row r="23" spans="1:11" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>374</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C23" s="48" t="s">
-        <v>435</v>
+      <c r="C23" s="12" t="s">
+        <v>432</v>
       </c>
       <c r="D23" s="30" t="s">
         <v>340</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>437</v>
-      </c>
-      <c r="H23" s="12"/>
+        <v>491</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>492</v>
+      </c>
       <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="12"/>
+      <c r="J23" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
@@ -9593,322 +9753,401 @@
       <c r="B24" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C24" s="48" t="s">
-        <v>438</v>
+      <c r="C24" s="12" t="s">
+        <v>434</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>340</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="H24" s="12"/>
+        <v>436</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>494</v>
+      </c>
       <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
+      <c r="J24" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>376</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C25" s="48" t="s">
-        <v>441</v>
+      <c r="C25" s="12" t="s">
+        <v>437</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>340</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>421</v>
+        <v>438</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="H25" s="12"/>
+        <v>439</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>495</v>
+      </c>
       <c r="I25" s="14"/>
-      <c r="J25" s="28"/>
+      <c r="J25" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>380</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C26" s="48" t="s">
-        <v>444</v>
+      <c r="C26" s="12" t="s">
+        <v>440</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>340</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>445</v>
+        <v>421</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>446</v>
-      </c>
-      <c r="H26" s="12"/>
+        <v>462</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>496</v>
+      </c>
       <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
+      <c r="J26" s="40" t="s">
+        <v>134</v>
+      </c>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>381</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C27" s="48" t="s">
-        <v>447</v>
+      <c r="C27" s="12" t="s">
+        <v>443</v>
       </c>
       <c r="D27" s="30" t="s">
         <v>340</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="H27" s="12"/>
+        <v>445</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>497</v>
+      </c>
       <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="J27" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>382</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C28" s="48" t="s">
-        <v>389</v>
+      <c r="C28" s="12" t="s">
+        <v>446</v>
       </c>
       <c r="D28" s="30" t="s">
         <v>340</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>455</v>
-      </c>
-      <c r="F28" s="47" t="s">
-        <v>190</v>
+        <v>447</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="H28" s="12"/>
+        <v>448</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>498</v>
+      </c>
       <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
+      <c r="J28" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>383</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C29" s="48" t="s">
-        <v>450</v>
-      </c>
-      <c r="D29" s="30"/>
+      <c r="C29" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>340</v>
+      </c>
       <c r="E29" s="12" t="s">
-        <v>451</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>471</v>
+        <v>454</v>
+      </c>
+      <c r="F29" s="43" t="s">
+        <v>190</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>452</v>
-      </c>
-      <c r="H29" s="12"/>
+        <v>448</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>498</v>
+      </c>
       <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
+      <c r="J29" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K29" s="12"/>
     </row>
-    <row r="30" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>384</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C30" s="48" t="s">
-        <v>388</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>340</v>
-      </c>
+      <c r="C30" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="D30" s="30"/>
       <c r="E30" s="12" t="s">
-        <v>453</v>
-      </c>
-      <c r="F30" s="47" t="s">
-        <v>190</v>
+        <v>450</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>470</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>454</v>
-      </c>
-      <c r="H30" s="12"/>
+        <v>451</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>451</v>
+      </c>
       <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
+      <c r="J30" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K30" s="12"/>
     </row>
-    <row r="31" spans="1:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>385</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C31" s="48" t="s">
-        <v>390</v>
+      <c r="C31" s="12" t="s">
+        <v>388</v>
       </c>
       <c r="D31" s="30" t="s">
         <v>340</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>456</v>
-      </c>
-      <c r="F31" s="47" t="s">
+        <v>452</v>
+      </c>
+      <c r="F31" s="43" t="s">
         <v>190</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>454</v>
-      </c>
-      <c r="H31" s="12"/>
+        <v>453</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>498</v>
+      </c>
       <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
+      <c r="J31" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K31" s="12"/>
     </row>
-    <row r="32" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>386</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C32" s="48" t="s">
-        <v>391</v>
+      <c r="C32" s="12" t="s">
+        <v>390</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>340</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>457</v>
-      </c>
-      <c r="F32" s="47" t="s">
+        <v>455</v>
+      </c>
+      <c r="F32" s="43" t="s">
         <v>190</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>454</v>
-      </c>
-      <c r="H32" s="12"/>
+        <v>453</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>498</v>
+      </c>
       <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
+      <c r="J32" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="1:11" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>387</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C33" s="48" t="s">
-        <v>392</v>
+      <c r="C33" s="12" t="s">
+        <v>391</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>340</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>458</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>471</v>
-      </c>
-      <c r="G33" s="30" t="s">
-        <v>462</v>
-      </c>
-      <c r="H33" s="12"/>
+        <v>456</v>
+      </c>
+      <c r="F33" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>498</v>
+      </c>
       <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
+      <c r="J33" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K33" s="12"/>
     </row>
-    <row r="34" spans="1:11" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>393</v>
+      <c r="C34" s="12" t="s">
+        <v>392</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>340</v>
       </c>
-      <c r="E34" s="46" t="s">
-        <v>459</v>
+      <c r="E34" s="12" t="s">
+        <v>457</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>460</v>
-      </c>
-      <c r="H34" s="12"/>
+        <v>461</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>499</v>
+      </c>
       <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
+      <c r="J34" s="41" t="s">
+        <v>78</v>
+      </c>
       <c r="K34" s="12"/>
     </row>
-    <row r="35" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="C35" s="49" t="s">
-        <v>394</v>
+      <c r="C35" s="12" t="s">
+        <v>393</v>
       </c>
       <c r="D35" s="30" t="s">
         <v>340</v>
       </c>
-      <c r="E35" s="12" t="s">
-        <v>461</v>
+      <c r="E35" s="42" t="s">
+        <v>458</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G35" s="30" t="s">
+        <v>459</v>
+      </c>
+      <c r="H35" s="30" t="s">
+        <v>500</v>
+      </c>
+      <c r="I35" s="14"/>
+      <c r="J35" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="K35" s="12"/>
+    </row>
+    <row r="36" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>460</v>
       </c>
-      <c r="H35" s="12"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="12"/>
-    </row>
-    <row r="36" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F36" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="G36" s="30" t="s">
+        <v>459</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>500</v>
+      </c>
+      <c r="I36" s="14"/>
+      <c r="J36" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="K36" s="12"/>
+    </row>
+    <row r="37" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9920,7 +10159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94942F9E-45C7-4B29-83B5-1A2A1569DC17}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implement Forgot Password Testing
</commit_message>
<xml_diff>
--- a/Test Cases of pickaboo.com(Full & Final ).xlsx
+++ b/Test Cases of pickaboo.com(Full & Final ).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SQA2\Projects\Test Cases of pickaboo.com(Full &amp; Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4832FFDF-3978-41C1-B80D-2168BDE41089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDC1FB0-EE53-4683-B361-A8E7B17B6093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="796" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="628">
   <si>
     <t>Project Name</t>
   </si>
@@ -3165,6 +3165,455 @@
   </si>
   <si>
     <t>TC_PD_030</t>
+  </si>
+  <si>
+    <t>TC_FP_001</t>
+  </si>
+  <si>
+    <t>(TS_004)
+Forgot Passsword</t>
+  </si>
+  <si>
+    <t>Verify User is able to reset the password</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL and navigate to Login Page
+2. An existing Account is required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on 'Forgotten Password' link from Login page (Verify ER-1)
+2. Enter the email address of an existing account for which you have forgot the password 
+3. Click on 'Continue' button (Verify ER-2)
+4. Check the registered email address for which the password got reset (Verify ER-3)
+5. Click on the link for resseting the password from the received email body (Verify ER-4)
+6. Enter new password into the 'Password' and 'Confirm' fields
+7. Click on 'Continue' button (Verify ER-5)
+8. Enter the email address into the E-Mail address field and the new resetted password into the 'Password' field 
+9. Click on 'Login' button (Verify ER-6)
+</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Forgotten Password' page
+2. Success message with text - 'An email with a confirmation link has been sent your email address.' should be displayed in green color
+3. Verify that an email is received regarding resseting of the password to the registered email address 
+4. User should be taken 'Reset your Password' page
+5. Success message with text - 'Success: Your password has been successfully updated.' should be displayed in green color and User should be navigated to 'Login' page
+6. User should be able to login with the new password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Application Email system is not working </t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Blocked</t>
+  </si>
+  <si>
+    <t>Unable to test as the application email system in not working due to the defect# TU1-I2</t>
+  </si>
+  <si>
+    <t>TC_FP_002</t>
+  </si>
+  <si>
+    <t>Verify an email is sent with the proper details on resetting the password</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page 
+2. Enter the email address of an existing account for which you have forgot the password 
+3. Click on 'Continue' button
+4. Check the registered email address for which the password got reset (Verify ER-1 and ER-2)</t>
+  </si>
+  <si>
+    <t>1. An email should be recevied by the registered email address with the details of resetting the password.
+2. Email should contain proper Subject, Body, from address and the link for resetting the password</t>
+  </si>
+  <si>
+    <t>TC_FP_003</t>
+  </si>
+  <si>
+    <t>Verify logging into the Application with the old password after resetting it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. An existing Account is required and we have reset the password
+2. Open the Application URL and navigate to Login Page
+</t>
+  </si>
+  <si>
+    <t>1. Enter registered email address into the 'E-Mail address' field
+2. Enter new password into the 'Password' field
+3. Click on 'Login' button (Verify ER-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User should not be able to login with old password </t>
+  </si>
+  <si>
+    <t>TC_FP_004</t>
+  </si>
+  <si>
+    <t>Verify logging into the Application with the old password when you have initiated the resetting password process and have not reset the password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL and navigate to Login Page
+1. An existing Account is required 
+</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Enter the email address of an existing account for which you have forgot the password 
+3. Click on 'Continue' button
+4. Enter registered email address into the 'E-mail Address' field
+5. Enter old password into the 'Password' field
+6. Click on 'Login' button</t>
+  </si>
+  <si>
+    <t>1. User should be able to login</t>
+  </si>
+  <si>
+    <t>TC_FP_005</t>
+  </si>
+  <si>
+    <t>Verify resetting the password for a non-registered account</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL and navigate to Login Page</t>
+  </si>
+  <si>
+    <t>1.Click on 'Forgotten Password' link from Login page
+2. Enter an email address for which the Account doesn't exist in the application
+3. Click on 'Continue' button</t>
+  </si>
+  <si>
+    <t>1. Success message with text - 'An email with a confirmation link has been sent your email address.' should be displayed in green color</t>
+  </si>
+  <si>
+    <t>1. Success message with text - 'An email with a confirmation link has been sent your email address.' is displayed in green color</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>TC_FP_006</t>
+  </si>
+  <si>
+    <t>Verify how many times the User is able to reset the password using the reset link sent over email</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Enter the email address of an existing account for which you have forgot the password 
+3. Click on 'Continue' button
+4. Check the registered email address for which the password got reset 
+5. Click on the link for resseting the password from the received email body
+6. Enter new password into the 'Password' and 'Confirm' fields
+7. Click on 'Continue' button 
+8. Repeat steps 5 to 7  for 2 to 3 times (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be allowed to use the link sent in the email for resetting the password only once</t>
+  </si>
+  <si>
+    <t>TC_FP_007</t>
+  </si>
+  <si>
+    <t>Verify the User has given the same password into the 'Password' and 'Confirm' fields of the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Enter the email address of an existing account for which you have forgot the password 
+3. Click on 'Continue' button
+4. Check the registered email address for which the password got reset 
+5. Click on the link for resseting the password from the received email body
+6. Enter a password into the 'Password' field 
+7. Enter a different password into the 'Confirm' fields
+8. Click on 'Continue' button (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. A field level warning message with text - 'Password and password confirmation do not match!' should be displayed under 'confirm' field</t>
+  </si>
+  <si>
+    <t>TC_FP_008</t>
+  </si>
+  <si>
+    <t>Verify the placeholders are displayed in the 'Password' and 'Confirm' fields of 'Reset your password' page</t>
+  </si>
+  <si>
+    <t>1. An existing Account is required, we have reset the password for this account and a reset password email is sent to the registered email address</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Check whether the 'Password' and 'Confirm' fields in the 'Reset your Password' page (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper placeholder texts are displayed inside the 'Password' and 'Confirm' fields of the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>TC_FP_009</t>
+  </si>
+  <si>
+    <t>Verify resetting the password without giving the new password in the 'Password' and 'Confirm' fields of 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Don't enter any password into the 'Password' and 'Confirm' fields of the 'Reset your Password' page
+3. Click on 'Continue' button (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Field level warning message with text - 'Password must be between 4 and 20 characters!' should be displayed for 'Password' field</t>
+  </si>
+  <si>
+    <t>TC_FP_010</t>
+  </si>
+  <si>
+    <t>Verify clicking  'Back' button on the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Click on 'Back' button on the 'Reset your Password' page (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to 'Login' page</t>
+  </si>
+  <si>
+    <t>TC_FP_011</t>
+  </si>
+  <si>
+    <t>Verify 'Right Column' options are displayed in the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Check for 'Right Column' options (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. 'Right Columns' options should be displayed in the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_012</t>
+  </si>
+  <si>
+    <t>Verify the Breadcrumb of the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Check the Breadcrumb (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. A proper working Breadcrumb should be displayed on the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_013</t>
+  </si>
+  <si>
+    <t>Verify Page Heading, Page URL and Page Title of the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Check the Page Heading, Page URL and Page Title (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. A proper Page Heading, Page URL and Page Title should be displayed for 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_014</t>
+  </si>
+  <si>
+    <t>Verify the UI of the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Check the UI of the Page (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_015</t>
+  </si>
+  <si>
+    <t>Verify reseting the Password without providing the registered email address</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Don't enter anything into the 'E-Mail Address' field
+3. Click on 'Continue' button (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Field level warning message with text - E-Mail must be between 4 and 20 characters!' should be displayed for 'E-Mail Address' field</t>
+  </si>
+  <si>
+    <t>1. Field level warning message with text - E-Mail must be between 4 and 20 characters!' is displayed for 'E-Mail Address' field</t>
+  </si>
+  <si>
+    <t>TC_FP_016</t>
+  </si>
+  <si>
+    <t>Verifty Placehold text is displayed in the 'E-Mail Address' field of 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Check  Placeholder text for 'E-Mail' Address field (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper Placeholder text should be displayed inside the 'E-Mail Address' fields  of the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Proper Placeholder text is displayed inside the 'E-Mail Address' fields  of the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_017</t>
+  </si>
+  <si>
+    <t>Verify 'E-Mail Address' fied on the 'Forgotten Password' page is marked as mandatory</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Check  the 'E-Mail' Address field (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. 'E-Mail' Address field in the 'Forgotten Password' page should be marked as mandatory</t>
+  </si>
+  <si>
+    <t>1. 'E-Mail' Address field in the 'Forgotten Password' page is marked as mandatory</t>
+  </si>
+  <si>
+    <t>TC_FP_018</t>
+  </si>
+  <si>
+    <t>Verify entering invalid format email address into the 'E-Mail Address' field of 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Enter any invalid formatted email address into the 'E-Mail Address' field (Verify ER-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try all below invalid email address formats:
+1) amotoori
+2) amotoori@
+3) amotoori@gmail
+4) amotoori@gmail.
+</t>
+  </si>
+  <si>
+    <t>1. Field level warning message informing the User to provide a valid formatted email address should be displayed</t>
+  </si>
+  <si>
+    <t>1. Field level warning message informing the User to provide a valid formatted email address is displayed</t>
+  </si>
+  <si>
+    <t>TC_FP_019</t>
+  </si>
+  <si>
+    <t>Verify Back button on the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Click on 'Back' button  (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Login' page</t>
+  </si>
+  <si>
+    <t>1. User is taken to 'Login' page</t>
+  </si>
+  <si>
+    <t>TC_FP_020</t>
+  </si>
+  <si>
+    <t>Verify navigating to 'Forgotten Password' page from 'Right Column' options</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' option from the 'Right Column'  (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to 'Forgotten Password page</t>
+  </si>
+  <si>
+    <t>1. User is navigated to 'Forgotten Password page</t>
+  </si>
+  <si>
+    <t>TC_FP_021</t>
+  </si>
+  <si>
+    <t>Verify Breadcrumb of the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Check the working of Breadcrumb (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. A proper working Breadcrumb should be displayed on the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. A proper working Breadcrumb is  displayed on the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_022</t>
+  </si>
+  <si>
+    <t>Verify the email address provided in the 'E-Mail Address' field of 'Login' page, need to be carry forwarded to the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Enter email address into the 'E-Mail Address' field of the Login page
+2. Click on 'Forgotten Password' link (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Forgotten Password' page and email address given in the Login page should be displayed in this page by default [Usability point of view]</t>
+  </si>
+  <si>
+    <t>1. User is taken to 'Forgotten Password' page and email address given in the Login page is not displayed in this page by default [Usability point of view]</t>
+  </si>
+  <si>
+    <t>Failed due to defect# TU1-I13</t>
+  </si>
+  <si>
+    <t>TC_FP_023</t>
+  </si>
+  <si>
+    <t>Verify the UI of the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Check the UI of the Page (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist is displayed for 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_024</t>
+  </si>
+  <si>
+    <t>Verify the Password entered into the 'Password' and 'Confirm' fields of 'Reset your Password' page is toggled to hide its visibility</t>
+  </si>
+  <si>
+    <t>1. An existing Account is required, we have reset the D1:D25password for this account and a reset password email is sent to the registered email address</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Enter any text into 'Password' and 'Confirm' fields on the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Text entered into the 'Password' and 'Confirmed' fields should be toggled to hide its visibility (i.e. * or . Symbols should be displayed)</t>
+  </si>
+  <si>
+    <t>TC_FP_025</t>
+  </si>
+  <si>
+    <t>Verify the Password Reset functionality in all the supported environments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL and navigate to Login Page
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on 'Forgotten Password' link from Login page </t>
+  </si>
+  <si>
+    <t>1. Reset Password functionality should work correctly in all the supported environments</t>
   </si>
 </sst>
 </file>
@@ -3364,7 +3813,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3507,6 +3956,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3514,7 +3976,36 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{39CB52D2-00E3-4F35-83F8-5B6A1156C826}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -8063,10 +8554,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1D6D1D-D934-49DC-940E-1A93D2F5E2D1}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8102,7 +8593,7 @@
       </c>
       <c r="J2" s="23">
         <f>COUNTIF(J7:J14, "Pass")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8135,7 +8626,7 @@
       </c>
       <c r="J5" s="23">
         <f>SUM(J2:J4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8174,253 +8665,882 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="12"/>
+      <c r="A7" s="48" t="s">
+        <v>502</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>504</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>506</v>
+      </c>
+      <c r="F7" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>507</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I7" s="48" t="s">
+        <v>509</v>
+      </c>
+      <c r="J7" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K7" s="30" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="12"/>
+      <c r="A8" s="48" t="s">
+        <v>512</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>513</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>514</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>515</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I8" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="12"/>
+      <c r="A9" s="48" t="s">
+        <v>516</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>517</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>518</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>519</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>520</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I9" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K9" s="30" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="12"/>
+      <c r="A10" s="48" t="s">
+        <v>521</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>522</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>523</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>524</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>525</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K10" s="30" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12"/>
+      <c r="A11" s="48" t="s">
+        <v>526</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>527</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>529</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>530</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>531</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="50" t="s">
+        <v>532</v>
+      </c>
+      <c r="K11" s="51"/>
     </row>
     <row r="12" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12"/>
+      <c r="A12" s="48" t="s">
+        <v>533</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>534</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>535</v>
+      </c>
+      <c r="F12" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>536</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K12" s="30" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12"/>
+      <c r="A13" s="48" t="s">
+        <v>537</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>538</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>539</v>
+      </c>
+      <c r="F13" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>540</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K13" s="30" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12"/>
+      <c r="A14" s="48" t="s">
+        <v>541</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>542</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>543</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>544</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>545</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I14" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J14" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K14" s="30" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="12"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="12"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="12"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="12"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="12"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="12"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="12"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="12"/>
+      <c r="A15" s="48" t="s">
+        <v>547</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>548</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>543</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>549</v>
+      </c>
+      <c r="F15" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>550</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I15" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J15" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K15" s="30" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="48" t="s">
+        <v>551</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>552</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>543</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>553</v>
+      </c>
+      <c r="F16" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>554</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I16" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J16" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K16" s="30" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="48" t="s">
+        <v>555</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>556</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>543</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>557</v>
+      </c>
+      <c r="F17" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>558</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I17" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J17" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K17" s="30" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="48" t="s">
+        <v>559</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>560</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>543</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>561</v>
+      </c>
+      <c r="F18" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>562</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I18" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J18" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K18" s="30" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="48" t="s">
+        <v>563</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>564</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>543</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>565</v>
+      </c>
+      <c r="F19" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>566</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I19" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J19" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K19" s="30" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="48" t="s">
+        <v>567</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>568</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>543</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>569</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>570</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I20" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J20" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K20" s="30" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>572</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>573</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>574</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>575</v>
+      </c>
+      <c r="I21" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J21" s="50" t="s">
+        <v>532</v>
+      </c>
+      <c r="K21" s="51"/>
+    </row>
+    <row r="22" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="48" t="s">
+        <v>576</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>577</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>578</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>579</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>580</v>
+      </c>
+      <c r="I22" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J22" s="50" t="s">
+        <v>532</v>
+      </c>
+      <c r="K22" s="51"/>
+    </row>
+    <row r="23" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
+        <v>581</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>582</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>583</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>584</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>585</v>
+      </c>
+      <c r="I23" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J23" s="50" t="s">
+        <v>532</v>
+      </c>
+      <c r="K23" s="51"/>
+    </row>
+    <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
+        <v>586</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>587</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>588</v>
+      </c>
+      <c r="F24" s="52" t="s">
+        <v>589</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>590</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>591</v>
+      </c>
+      <c r="I24" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J24" s="50" t="s">
+        <v>532</v>
+      </c>
+      <c r="K24" s="51"/>
+    </row>
+    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="48" t="s">
+        <v>592</v>
+      </c>
+      <c r="B25" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>593</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>594</v>
+      </c>
+      <c r="F25" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>595</v>
+      </c>
+      <c r="H25" s="30" t="s">
+        <v>596</v>
+      </c>
+      <c r="I25" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J25" s="50" t="s">
+        <v>532</v>
+      </c>
+      <c r="K25" s="51"/>
+    </row>
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="48" t="s">
+        <v>597</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>598</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>599</v>
+      </c>
+      <c r="F26" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>600</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>601</v>
+      </c>
+      <c r="I26" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J26" s="50" t="s">
+        <v>532</v>
+      </c>
+      <c r="K26" s="51"/>
+    </row>
+    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="48" t="s">
+        <v>602</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>603</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>604</v>
+      </c>
+      <c r="F27" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>605</v>
+      </c>
+      <c r="H27" s="30" t="s">
+        <v>606</v>
+      </c>
+      <c r="I27" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J27" s="50" t="s">
+        <v>532</v>
+      </c>
+      <c r="K27" s="51"/>
+    </row>
+    <row r="28" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A28" s="48" t="s">
+        <v>607</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>608</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>609</v>
+      </c>
+      <c r="F28" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G28" s="30" t="s">
+        <v>610</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>611</v>
+      </c>
+      <c r="I28" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J28" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="K28" s="30" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="48" t="s">
+        <v>613</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>614</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>615</v>
+      </c>
+      <c r="F29" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G29" s="30" t="s">
+        <v>616</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>617</v>
+      </c>
+      <c r="I29" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="J29" s="50" t="s">
+        <v>532</v>
+      </c>
+      <c r="K29" s="51"/>
+    </row>
+    <row r="30" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A30" s="48" t="s">
+        <v>618</v>
+      </c>
+      <c r="B30" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>619</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>620</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>621</v>
+      </c>
+      <c r="F30" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G30" s="30" t="s">
+        <v>622</v>
+      </c>
+      <c r="H30" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I30" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K30" s="30" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="48" t="s">
+        <v>623</v>
+      </c>
+      <c r="B31" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>624</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>625</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>626</v>
+      </c>
+      <c r="F31" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>627</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="I31" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="50" t="s">
+        <v>510</v>
+      </c>
+      <c r="K31" s="30" t="s">
+        <v>511</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J7:J31">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:J31" xr:uid="{1CDF2FDA-FD8D-4A7B-9C6E-E38B6558C75B}">
+      <formula1>"PASS, FAIL, Blocked, Not Tested"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement my account testing
</commit_message>
<xml_diff>
--- a/Test Cases of pickaboo.com(Full & Final ).xlsx
+++ b/Test Cases of pickaboo.com(Full & Final ).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SQA2\Projects\Test Cases of pickaboo.com(Full &amp; Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDC1FB0-EE53-4683-B361-A8E7B17B6093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7014D61-14A6-4F87-8F53-42483E276A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="796" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="796" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="669">
   <si>
     <t>Project Name</t>
   </si>
@@ -3614,6 +3614,143 @@
   </si>
   <si>
     <t>1. Reset Password functionality should work correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t>TC_MA_001</t>
+  </si>
+  <si>
+    <t>(TS_013)
+My Account</t>
+  </si>
+  <si>
+    <t>Verify navigating to 'My Account' page from the 'Order Success' page</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL, login and place an order for a product  - &lt;Refer Test Data&gt;</t>
+  </si>
+  <si>
+    <t>1. Click on 'my account' page link in the displayed 'Order Success' page (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>Product Name: iMac</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'My Account' page</t>
+  </si>
+  <si>
+    <t>Working as mentioned in the Expected Result section</t>
+  </si>
+  <si>
+    <t>TC_MA_002</t>
+  </si>
+  <si>
+    <t>Verify navigating to 'My Account' page on login</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Dropmenu
+2. Click on 'Login' option 
+3. Enter valid email address into the 'E-Mail Address' field - &lt;Refer Test Data&gt;
+4. Enter valid password into the 'Password' field - &lt;Refer Test Data&gt;
+5. Click on 'Login' button (Verify ER-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Address - amotoori3@gmail.com
+Password -
+12345
+</t>
+  </si>
+  <si>
+    <t>1. User should be able to login and taken to 'My Account' page</t>
+  </si>
+  <si>
+    <t>TC_MA_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify navigating to 'My Account' page using 'My Account' option </t>
+  </si>
+  <si>
+    <t>1. Open the Application URL and login</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' dropmenu
+2. Click on 'My Account' option (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>TC_MA_004</t>
+  </si>
+  <si>
+    <t>Verify navigating to 'My Account' page using 'Right Column' options</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' option from any page say 'Order History' page (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>TC_MA_005</t>
+  </si>
+  <si>
+    <t>Verify navigating to 'My Account' page using 'My Account' option in Site Map page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Site Map' link in the Footer options
+2. Click on 'My Account' link in the displayed 'Site Map' page (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>TC_MA_006</t>
+  </si>
+  <si>
+    <t>Verify Breadcrump in 'My Account' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' dropmenu
+2. Click on 'My Account' option
+3. Verify the Breadcrumb in the displayed 'My Account' page</t>
+  </si>
+  <si>
+    <t>1. Breadcrumb should be displayed in the 'My Account' page and is working properly</t>
+  </si>
+  <si>
+    <t>TC_MA_007</t>
+  </si>
+  <si>
+    <t>Verify Page URL, Page Heading and Page Title of the 'My Account' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' dropmenu
+2. Click on 'My Account' option
+3. Check the Page URL, Page Title and Page Heading that is displayed in the 'My Account' page (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Correct Page URL, Page Title and Page Heading should be displayed</t>
+  </si>
+  <si>
+    <t>TC_MA_008</t>
+  </si>
+  <si>
+    <t>Verify the UI of 'My Account' page functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL in any supported browser </t>
+  </si>
+  <si>
+    <t>1. Check the UI of the functionality related to 'My Account' page  (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for the 'My Account' page functionality</t>
+  </si>
+  <si>
+    <t>TC_MA_009</t>
+  </si>
+  <si>
+    <t>Verify the 'My Account' page functionality in all the supported environments</t>
+  </si>
+  <si>
+    <t>1. Check the 'My Account' page functionality in all the supported environments (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. 'My Account' page functionality should work correctly in all the supported environments</t>
   </si>
 </sst>
 </file>
@@ -3944,18 +4081,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3969,6 +4094,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3976,7 +4113,349 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{39CB52D2-00E3-4F35-83F8-5B6A1156C826}"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4295,10 +4774,10 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="45"/>
+      <c r="C6" s="50"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -4319,7 +4798,7 @@
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="49" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -4328,17 +4807,17 @@
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="44"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="44"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
@@ -6203,56 +6682,56 @@
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="46"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="47"/>
+      <c r="E3" s="52"/>
     </row>
     <row r="4" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
     </row>
     <row r="5" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46"/>
+      <c r="E5" s="51"/>
     </row>
     <row r="6" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="46"/>
+      <c r="E6" s="51"/>
     </row>
     <row r="7" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
@@ -8556,7 +9035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1D6D1D-D934-49DC-940E-1A93D2F5E2D1}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -8665,10 +9144,10 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="44" t="s">
         <v>502</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C7" s="30" t="s">
@@ -8680,7 +9159,7 @@
       <c r="E7" s="30" t="s">
         <v>506</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G7" s="30" t="s">
@@ -8689,10 +9168,10 @@
       <c r="H7" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I7" s="48" t="s">
+      <c r="I7" s="44" t="s">
         <v>509</v>
       </c>
-      <c r="J7" s="50" t="s">
+      <c r="J7" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K7" s="30" t="s">
@@ -8700,10 +9179,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="44" t="s">
         <v>512</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C8" s="30" t="s">
@@ -8715,7 +9194,7 @@
       <c r="E8" s="30" t="s">
         <v>514</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G8" s="30" t="s">
@@ -8724,10 +9203,10 @@
       <c r="H8" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="50" t="s">
+      <c r="J8" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K8" s="30" t="s">
@@ -8735,10 +9214,10 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="44" t="s">
         <v>516</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C9" s="30" t="s">
@@ -8750,7 +9229,7 @@
       <c r="E9" s="30" t="s">
         <v>519</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G9" s="30" t="s">
@@ -8759,10 +9238,10 @@
       <c r="H9" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I9" s="48" t="s">
+      <c r="I9" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="50" t="s">
+      <c r="J9" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K9" s="30" t="s">
@@ -8770,10 +9249,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="44" t="s">
         <v>521</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C10" s="30" t="s">
@@ -8785,7 +9264,7 @@
       <c r="E10" s="30" t="s">
         <v>524</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="F10" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G10" s="30" t="s">
@@ -8794,10 +9273,10 @@
       <c r="H10" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K10" s="30" t="s">
@@ -8805,10 +9284,10 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="44" t="s">
         <v>526</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C11" s="30" t="s">
@@ -8820,7 +9299,7 @@
       <c r="E11" s="30" t="s">
         <v>529</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G11" s="30" t="s">
@@ -8829,19 +9308,19 @@
       <c r="H11" s="30" t="s">
         <v>531</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="50" t="s">
+      <c r="J11" s="46" t="s">
         <v>532</v>
       </c>
-      <c r="K11" s="51"/>
+      <c r="K11" s="47"/>
     </row>
     <row r="12" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="44" t="s">
         <v>533</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C12" s="30" t="s">
@@ -8853,7 +9332,7 @@
       <c r="E12" s="30" t="s">
         <v>535</v>
       </c>
-      <c r="F12" s="49" t="s">
+      <c r="F12" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G12" s="30" t="s">
@@ -8862,10 +9341,10 @@
       <c r="H12" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I12" s="48" t="s">
+      <c r="I12" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="50" t="s">
+      <c r="J12" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K12" s="30" t="s">
@@ -8873,10 +9352,10 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="44" t="s">
         <v>537</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C13" s="30" t="s">
@@ -8888,7 +9367,7 @@
       <c r="E13" s="30" t="s">
         <v>539</v>
       </c>
-      <c r="F13" s="49" t="s">
+      <c r="F13" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G13" s="30" t="s">
@@ -8897,10 +9376,10 @@
       <c r="H13" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I13" s="48" t="s">
+      <c r="I13" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="50" t="s">
+      <c r="J13" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K13" s="30" t="s">
@@ -8908,10 +9387,10 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="44" t="s">
         <v>541</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C14" s="30" t="s">
@@ -8923,7 +9402,7 @@
       <c r="E14" s="30" t="s">
         <v>544</v>
       </c>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G14" s="30" t="s">
@@ -8932,10 +9411,10 @@
       <c r="H14" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I14" s="48" t="s">
+      <c r="I14" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J14" s="50" t="s">
+      <c r="J14" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K14" s="30" t="s">
@@ -8943,10 +9422,10 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="44" t="s">
         <v>547</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C15" s="30" t="s">
@@ -8958,7 +9437,7 @@
       <c r="E15" s="30" t="s">
         <v>549</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G15" s="30" t="s">
@@ -8967,10 +9446,10 @@
       <c r="H15" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I15" s="48" t="s">
+      <c r="I15" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J15" s="50" t="s">
+      <c r="J15" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K15" s="30" t="s">
@@ -8978,10 +9457,10 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="44" t="s">
         <v>551</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C16" s="30" t="s">
@@ -8993,7 +9472,7 @@
       <c r="E16" s="30" t="s">
         <v>553</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G16" s="30" t="s">
@@ -9002,10 +9481,10 @@
       <c r="H16" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I16" s="48" t="s">
+      <c r="I16" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J16" s="50" t="s">
+      <c r="J16" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K16" s="30" t="s">
@@ -9013,10 +9492,10 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="44" t="s">
         <v>555</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C17" s="30" t="s">
@@ -9028,7 +9507,7 @@
       <c r="E17" s="30" t="s">
         <v>557</v>
       </c>
-      <c r="F17" s="49" t="s">
+      <c r="F17" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G17" s="30" t="s">
@@ -9037,10 +9516,10 @@
       <c r="H17" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I17" s="48" t="s">
+      <c r="I17" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J17" s="50" t="s">
+      <c r="J17" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K17" s="30" t="s">
@@ -9048,10 +9527,10 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="44" t="s">
         <v>559</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C18" s="30" t="s">
@@ -9063,7 +9542,7 @@
       <c r="E18" s="30" t="s">
         <v>561</v>
       </c>
-      <c r="F18" s="49" t="s">
+      <c r="F18" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G18" s="30" t="s">
@@ -9072,10 +9551,10 @@
       <c r="H18" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I18" s="48" t="s">
+      <c r="I18" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J18" s="50" t="s">
+      <c r="J18" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K18" s="30" t="s">
@@ -9083,10 +9562,10 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="44" t="s">
         <v>563</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C19" s="30" t="s">
@@ -9098,7 +9577,7 @@
       <c r="E19" s="30" t="s">
         <v>565</v>
       </c>
-      <c r="F19" s="49" t="s">
+      <c r="F19" s="45" t="s">
         <v>190</v>
       </c>
       <c r="G19" s="30" t="s">
@@ -9107,10 +9586,10 @@
       <c r="H19" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I19" s="48" t="s">
+      <c r="I19" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J19" s="50" t="s">
+      <c r="J19" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K19" s="30" t="s">
@@ -9118,10 +9597,10 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="44" t="s">
         <v>567</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C20" s="30" t="s">
@@ -9133,7 +9612,7 @@
       <c r="E20" s="30" t="s">
         <v>569</v>
       </c>
-      <c r="F20" s="48" t="s">
+      <c r="F20" s="44" t="s">
         <v>190</v>
       </c>
       <c r="G20" s="30" t="s">
@@ -9142,10 +9621,10 @@
       <c r="H20" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I20" s="48" t="s">
+      <c r="I20" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J20" s="50" t="s">
+      <c r="J20" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K20" s="30" t="s">
@@ -9153,10 +9632,10 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="44" t="s">
         <v>571</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C21" s="30" t="s">
@@ -9168,7 +9647,7 @@
       <c r="E21" s="30" t="s">
         <v>573</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="F21" s="44" t="s">
         <v>190</v>
       </c>
       <c r="G21" s="30" t="s">
@@ -9177,19 +9656,19 @@
       <c r="H21" s="30" t="s">
         <v>575</v>
       </c>
-      <c r="I21" s="48" t="s">
+      <c r="I21" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J21" s="50" t="s">
+      <c r="J21" s="46" t="s">
         <v>532</v>
       </c>
-      <c r="K21" s="51"/>
+      <c r="K21" s="47"/>
     </row>
     <row r="22" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="44" t="s">
         <v>576</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C22" s="30" t="s">
@@ -9201,7 +9680,7 @@
       <c r="E22" s="30" t="s">
         <v>578</v>
       </c>
-      <c r="F22" s="48" t="s">
+      <c r="F22" s="44" t="s">
         <v>190</v>
       </c>
       <c r="G22" s="30" t="s">
@@ -9210,19 +9689,19 @@
       <c r="H22" s="30" t="s">
         <v>580</v>
       </c>
-      <c r="I22" s="48" t="s">
+      <c r="I22" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J22" s="50" t="s">
+      <c r="J22" s="46" t="s">
         <v>532</v>
       </c>
-      <c r="K22" s="51"/>
+      <c r="K22" s="47"/>
     </row>
     <row r="23" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="44" t="s">
         <v>581</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C23" s="30" t="s">
@@ -9234,7 +9713,7 @@
       <c r="E23" s="30" t="s">
         <v>583</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="44" t="s">
         <v>190</v>
       </c>
       <c r="G23" s="30" t="s">
@@ -9243,19 +9722,19 @@
       <c r="H23" s="30" t="s">
         <v>585</v>
       </c>
-      <c r="I23" s="48" t="s">
+      <c r="I23" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J23" s="50" t="s">
+      <c r="J23" s="46" t="s">
         <v>532</v>
       </c>
-      <c r="K23" s="51"/>
+      <c r="K23" s="47"/>
     </row>
     <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="44" t="s">
         <v>586</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C24" s="30" t="s">
@@ -9267,7 +9746,7 @@
       <c r="E24" s="30" t="s">
         <v>588</v>
       </c>
-      <c r="F24" s="52" t="s">
+      <c r="F24" s="48" t="s">
         <v>589</v>
       </c>
       <c r="G24" s="30" t="s">
@@ -9276,19 +9755,19 @@
       <c r="H24" s="30" t="s">
         <v>591</v>
       </c>
-      <c r="I24" s="48" t="s">
+      <c r="I24" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J24" s="50" t="s">
+      <c r="J24" s="46" t="s">
         <v>532</v>
       </c>
-      <c r="K24" s="51"/>
+      <c r="K24" s="47"/>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="44" t="s">
         <v>592</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C25" s="30" t="s">
@@ -9300,7 +9779,7 @@
       <c r="E25" s="30" t="s">
         <v>594</v>
       </c>
-      <c r="F25" s="48" t="s">
+      <c r="F25" s="44" t="s">
         <v>190</v>
       </c>
       <c r="G25" s="30" t="s">
@@ -9309,19 +9788,19 @@
       <c r="H25" s="30" t="s">
         <v>596</v>
       </c>
-      <c r="I25" s="48" t="s">
+      <c r="I25" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J25" s="50" t="s">
+      <c r="J25" s="46" t="s">
         <v>532</v>
       </c>
-      <c r="K25" s="51"/>
+      <c r="K25" s="47"/>
     </row>
     <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="44" t="s">
         <v>597</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C26" s="30" t="s">
@@ -9333,7 +9812,7 @@
       <c r="E26" s="30" t="s">
         <v>599</v>
       </c>
-      <c r="F26" s="48" t="s">
+      <c r="F26" s="44" t="s">
         <v>190</v>
       </c>
       <c r="G26" s="30" t="s">
@@ -9342,19 +9821,19 @@
       <c r="H26" s="30" t="s">
         <v>601</v>
       </c>
-      <c r="I26" s="48" t="s">
+      <c r="I26" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J26" s="50" t="s">
+      <c r="J26" s="46" t="s">
         <v>532</v>
       </c>
-      <c r="K26" s="51"/>
+      <c r="K26" s="47"/>
     </row>
     <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="44" t="s">
         <v>602</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C27" s="30" t="s">
@@ -9366,7 +9845,7 @@
       <c r="E27" s="30" t="s">
         <v>604</v>
       </c>
-      <c r="F27" s="48" t="s">
+      <c r="F27" s="44" t="s">
         <v>190</v>
       </c>
       <c r="G27" s="30" t="s">
@@ -9375,19 +9854,19 @@
       <c r="H27" s="30" t="s">
         <v>606</v>
       </c>
-      <c r="I27" s="48" t="s">
+      <c r="I27" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J27" s="50" t="s">
+      <c r="J27" s="46" t="s">
         <v>532</v>
       </c>
-      <c r="K27" s="51"/>
+      <c r="K27" s="47"/>
     </row>
     <row r="28" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="44" t="s">
         <v>607</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C28" s="30" t="s">
@@ -9399,7 +9878,7 @@
       <c r="E28" s="30" t="s">
         <v>609</v>
       </c>
-      <c r="F28" s="48" t="s">
+      <c r="F28" s="44" t="s">
         <v>190</v>
       </c>
       <c r="G28" s="30" t="s">
@@ -9408,10 +9887,10 @@
       <c r="H28" s="30" t="s">
         <v>611</v>
       </c>
-      <c r="I28" s="48" t="s">
+      <c r="I28" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J28" s="50" t="s">
+      <c r="J28" s="46" t="s">
         <v>98</v>
       </c>
       <c r="K28" s="30" t="s">
@@ -9419,10 +9898,10 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="44" t="s">
         <v>613</v>
       </c>
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C29" s="30" t="s">
@@ -9434,7 +9913,7 @@
       <c r="E29" s="30" t="s">
         <v>615</v>
       </c>
-      <c r="F29" s="48" t="s">
+      <c r="F29" s="44" t="s">
         <v>190</v>
       </c>
       <c r="G29" s="30" t="s">
@@ -9443,19 +9922,19 @@
       <c r="H29" s="30" t="s">
         <v>617</v>
       </c>
-      <c r="I29" s="48" t="s">
+      <c r="I29" s="44" t="s">
         <v>546</v>
       </c>
-      <c r="J29" s="50" t="s">
+      <c r="J29" s="46" t="s">
         <v>532</v>
       </c>
-      <c r="K29" s="51"/>
+      <c r="K29" s="47"/>
     </row>
     <row r="30" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="44" t="s">
         <v>618</v>
       </c>
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C30" s="30" t="s">
@@ -9467,7 +9946,7 @@
       <c r="E30" s="30" t="s">
         <v>621</v>
       </c>
-      <c r="F30" s="48" t="s">
+      <c r="F30" s="44" t="s">
         <v>190</v>
       </c>
       <c r="G30" s="30" t="s">
@@ -9476,10 +9955,10 @@
       <c r="H30" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I30" s="48" t="s">
+      <c r="I30" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="50" t="s">
+      <c r="J30" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K30" s="30" t="s">
@@ -9487,10 +9966,10 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="44" t="s">
         <v>623</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="45" t="s">
         <v>503</v>
       </c>
       <c r="C31" s="30" t="s">
@@ -9502,7 +9981,7 @@
       <c r="E31" s="30" t="s">
         <v>626</v>
       </c>
-      <c r="F31" s="48" t="s">
+      <c r="F31" s="44" t="s">
         <v>190</v>
       </c>
       <c r="G31" s="30" t="s">
@@ -9511,10 +9990,10 @@
       <c r="H31" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="I31" s="48" t="s">
+      <c r="I31" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J31" s="50" t="s">
+      <c r="J31" s="46" t="s">
         <v>510</v>
       </c>
       <c r="K31" s="30" t="s">
@@ -9523,16 +10002,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J7:J31">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="48" priority="1" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="47" priority="2" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="46" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="45" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",J7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11279,8 +11758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94942F9E-45C7-4B29-83B5-1A2A1569DC17}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11316,7 +11795,7 @@
       </c>
       <c r="J2" s="23">
         <f>COUNTIF(J7:J14, "Pass")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11349,7 +11828,7 @@
       </c>
       <c r="J5" s="23">
         <f>SUM(J2:J4)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11388,120 +11867,300 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="A7" s="44" t="s">
+        <v>628</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>629</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>630</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>631</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>632</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>633</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>634</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>635</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="J7" s="46" t="s">
+        <v>532</v>
+      </c>
       <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="A8" s="44" t="s">
+        <v>636</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>629</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>637</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>638</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>639</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>640</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>641</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>635</v>
+      </c>
+      <c r="I8" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="J8" s="46" t="s">
+        <v>532</v>
+      </c>
       <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="A9" s="44" t="s">
+        <v>642</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>629</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>643</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>644</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>645</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>634</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>635</v>
+      </c>
+      <c r="I9" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="J9" s="46" t="s">
+        <v>532</v>
+      </c>
       <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="A10" s="44" t="s">
+        <v>646</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>629</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>647</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>644</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>648</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>634</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>635</v>
+      </c>
+      <c r="I10" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="J10" s="46" t="s">
+        <v>532</v>
+      </c>
       <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="A11" s="44" t="s">
+        <v>649</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>629</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>650</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>644</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>651</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>634</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>635</v>
+      </c>
+      <c r="I11" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="J11" s="46" t="s">
+        <v>532</v>
+      </c>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="A12" s="44" t="s">
+        <v>652</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>629</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>653</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>644</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>654</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>655</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>635</v>
+      </c>
+      <c r="I12" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="J12" s="46" t="s">
+        <v>532</v>
+      </c>
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="A13" s="44" t="s">
+        <v>656</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>629</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>657</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>644</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>658</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>659</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>635</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="J13" s="46" t="s">
+        <v>532</v>
+      </c>
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="A14" s="44" t="s">
+        <v>660</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>629</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>661</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>662</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>663</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>664</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>635</v>
+      </c>
+      <c r="I14" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="J14" s="46" t="s">
+        <v>532</v>
+      </c>
       <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="A15" s="44" t="s">
+        <v>665</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>629</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>666</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>667</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>668</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>635</v>
+      </c>
+      <c r="I15" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="J15" s="46" t="s">
+        <v>532</v>
+      </c>
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -11635,6 +12294,164 @@
       <c r="K25" s="12"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H7:J7">
+    <cfRule type="duplicateValues" dxfId="44" priority="41"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:J8">
+    <cfRule type="duplicateValues" dxfId="43" priority="36"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:J9">
+    <cfRule type="duplicateValues" dxfId="42" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:J10">
+    <cfRule type="duplicateValues" dxfId="41" priority="26"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11:J11">
+    <cfRule type="duplicateValues" dxfId="40" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:J12">
+    <cfRule type="duplicateValues" dxfId="39" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13:J13">
+    <cfRule type="duplicateValues" dxfId="38" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:J14">
+    <cfRule type="duplicateValues" dxfId="37" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:J15">
+    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="containsText" dxfId="34" priority="42" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="44" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="45" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="containsText" dxfId="29" priority="37" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="38" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="39" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="40" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9">
+    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="33" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="34" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="35" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="25" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12">
+    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="19" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="20" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="10" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:J15" xr:uid="{5F687DBA-E22E-452D-B7F4-EF9E80D927AD}">
+      <formula1>"PASS, FAIL, Blocked, Not Tested"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>